<commit_message>
Research tab is ready.
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/FINDich.xlsx
+++ b/src/main/resources/templates/FINDich.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koko/IdeaProjects/FinanceProjects/stock-financial-report-analyzer/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0204853E-0AC8-A840-B043-B40B92337A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D54E391-3DDC-954F-A88C-B04D4447ED55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="76680" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="IS" sheetId="9" r:id="rId7"/>
     <sheet name="BS" sheetId="10" r:id="rId8"/>
     <sheet name="CF" sheetId="11" r:id="rId9"/>
-    <sheet name="RATIOS" sheetId="12" r:id="rId10"/>
+    <sheet name="RESEARCH" sheetId="13" r:id="rId10"/>
+    <sheet name="RATIOS" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="477">
   <si>
     <t>Ticker</t>
   </si>
@@ -1370,13 +1371,124 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Earnings Estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Year Ago EPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  High Estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Low Estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Avg. Estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  No. of Analysts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Revenue Estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Year Ago Sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Sales Growth (year/est)</t>
+  </si>
+  <si>
+    <t>Growth Estimates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Current Qtr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Next Qtr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Current Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Next Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Next 5 Years (per annum)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Past 5 Years (per annum)</t>
+  </si>
+  <si>
+    <t>Earnings History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  EPS Estimated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  EPS Actual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Surprise (%)</t>
+  </si>
+  <si>
+    <t>EPS Revisions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Up Last 7 Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Up Last 30 Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Down Last 7 Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Down Last 30 Days</t>
+  </si>
+  <si>
+    <t>EPS Trend</t>
+  </si>
+  <si>
+    <t>Current Quarter</t>
+  </si>
+  <si>
+    <t>Next Quarter</t>
+  </si>
+  <si>
+    <t>Current Year</t>
+  </si>
+  <si>
+    <t>Next Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Current Estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  7 Days Ago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  30 Days Ago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  60 Days Ago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  90 Days Ago</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="13">
+  <numFmts count="14">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="d&quot;-&quot;mmm&quot;-&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="[$$]#,##0.00"/>
@@ -1390,6 +1502,7 @@
     <numFmt numFmtId="174" formatCode="#,##0.0\x"/>
     <numFmt numFmtId="175" formatCode="#,##0.00\x"/>
     <numFmt numFmtId="176" formatCode="_(* #,##0.0#_);_(* \(#,##0.0#\)_)\ ;_(* 0_)"/>
+    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="49">
     <font>
@@ -1800,7 +1913,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -2210,6 +2323,113 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2217,7 +2437,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2634,6 +2854,42 @@
     <xf numFmtId="170" fontId="43" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="39" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="48" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2645,6 +2901,9 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2682,20 +2941,55 @@
     <xf numFmtId="0" fontId="39" fillId="9" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="171" fontId="32" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="32" fillId="0" borderId="45" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="172" fontId="32" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="32" fillId="0" borderId="45" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2764,7 +3058,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC53929"/>
+        <color rgb="FF0B8043"/>
       </font>
       <fill>
         <patternFill patternType="none"/>
@@ -2772,18 +3066,10 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF0B8043"/>
+        <color rgb="FFC53929"/>
       </font>
       <fill>
         <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
       </fill>
     </dxf>
     <dxf>
@@ -2803,8 +3089,16 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
-        <color rgb="FF7030A0"/>
+        <color rgb="FFC53929"/>
       </font>
       <fill>
         <patternFill patternType="none"/>
@@ -2812,7 +3106,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC53929"/>
+        <color rgb="FF7030A0"/>
       </font>
       <fill>
         <patternFill patternType="none"/>
@@ -3040,7 +3334,7 @@
   <dimension ref="B2:W41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3055,56 +3349,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" ht="15.75" customHeight="1">
-      <c r="B2" s="188" t="s">
+      <c r="B2" s="200" t="s">
         <v>431</v>
       </c>
-      <c r="C2" s="189"/>
-      <c r="D2" s="190" t="s">
+      <c r="C2" s="201"/>
+      <c r="D2" s="202" t="s">
         <v>432</v>
       </c>
-      <c r="E2" s="191"/>
-      <c r="F2" s="191"/>
-      <c r="G2" s="191"/>
-      <c r="H2" s="191"/>
-      <c r="I2" s="191"/>
-      <c r="J2" s="191"/>
-      <c r="K2" s="191"/>
-      <c r="L2" s="191"/>
-      <c r="M2" s="191"/>
-      <c r="N2" s="191"/>
-      <c r="O2" s="191"/>
-      <c r="P2" s="191"/>
-      <c r="Q2" s="191"/>
-      <c r="R2" s="191"/>
-      <c r="S2" s="191"/>
-      <c r="T2" s="191"/>
-      <c r="V2" s="188" t="s">
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="203"/>
+      <c r="H2" s="203"/>
+      <c r="I2" s="203"/>
+      <c r="J2" s="203"/>
+      <c r="K2" s="203"/>
+      <c r="L2" s="203"/>
+      <c r="M2" s="203"/>
+      <c r="N2" s="203"/>
+      <c r="O2" s="203"/>
+      <c r="P2" s="203"/>
+      <c r="Q2" s="203"/>
+      <c r="R2" s="203"/>
+      <c r="S2" s="203"/>
+      <c r="T2" s="203"/>
+      <c r="V2" s="200" t="s">
         <v>433</v>
       </c>
-      <c r="W2" s="189"/>
+      <c r="W2" s="201"/>
     </row>
     <row r="3" spans="2:23" ht="15">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="219"/>
-      <c r="E3" s="219"/>
-      <c r="F3" s="219"/>
-      <c r="G3" s="219"/>
-      <c r="H3" s="219"/>
-      <c r="I3" s="219"/>
-      <c r="J3" s="219"/>
-      <c r="K3" s="219"/>
-      <c r="L3" s="219"/>
-      <c r="M3" s="219"/>
-      <c r="N3" s="219"/>
-      <c r="O3" s="219"/>
-      <c r="P3" s="219"/>
-      <c r="Q3" s="219"/>
-      <c r="R3" s="219"/>
-      <c r="S3" s="219"/>
-      <c r="T3" s="219"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="204"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="204"/>
+      <c r="J3" s="204"/>
+      <c r="K3" s="204"/>
+      <c r="L3" s="204"/>
+      <c r="M3" s="204"/>
+      <c r="N3" s="204"/>
+      <c r="O3" s="204"/>
+      <c r="P3" s="204"/>
+      <c r="Q3" s="204"/>
+      <c r="R3" s="204"/>
+      <c r="S3" s="204"/>
+      <c r="T3" s="204"/>
       <c r="V3" s="3" t="s">
         <v>4</v>
       </c>
@@ -3116,24 +3410,24 @@
       <c r="B4" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="C4" s="218"/>
-      <c r="D4" s="219"/>
-      <c r="E4" s="219"/>
-      <c r="F4" s="219"/>
-      <c r="G4" s="219"/>
-      <c r="H4" s="219"/>
-      <c r="I4" s="219"/>
-      <c r="J4" s="219"/>
-      <c r="K4" s="219"/>
-      <c r="L4" s="219"/>
-      <c r="M4" s="219"/>
-      <c r="N4" s="219"/>
-      <c r="O4" s="219"/>
-      <c r="P4" s="219"/>
-      <c r="Q4" s="219"/>
-      <c r="R4" s="219"/>
-      <c r="S4" s="219"/>
-      <c r="T4" s="219"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="204"/>
+      <c r="E4" s="204"/>
+      <c r="F4" s="204"/>
+      <c r="G4" s="204"/>
+      <c r="H4" s="204"/>
+      <c r="I4" s="204"/>
+      <c r="J4" s="204"/>
+      <c r="K4" s="204"/>
+      <c r="L4" s="204"/>
+      <c r="M4" s="204"/>
+      <c r="N4" s="204"/>
+      <c r="O4" s="204"/>
+      <c r="P4" s="204"/>
+      <c r="Q4" s="204"/>
+      <c r="R4" s="204"/>
+      <c r="S4" s="204"/>
+      <c r="T4" s="204"/>
       <c r="V4" s="3"/>
       <c r="W4" s="4"/>
     </row>
@@ -3141,24 +3435,24 @@
       <c r="B5" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="C5" s="218"/>
-      <c r="D5" s="219"/>
-      <c r="E5" s="219"/>
-      <c r="F5" s="219"/>
-      <c r="G5" s="219"/>
-      <c r="H5" s="219"/>
-      <c r="I5" s="219"/>
-      <c r="J5" s="219"/>
-      <c r="K5" s="219"/>
-      <c r="L5" s="219"/>
-      <c r="M5" s="219"/>
-      <c r="N5" s="219"/>
-      <c r="O5" s="219"/>
-      <c r="P5" s="219"/>
-      <c r="Q5" s="219"/>
-      <c r="R5" s="219"/>
-      <c r="S5" s="219"/>
-      <c r="T5" s="219"/>
+      <c r="C5" s="188"/>
+      <c r="D5" s="204"/>
+      <c r="E5" s="204"/>
+      <c r="F5" s="204"/>
+      <c r="G5" s="204"/>
+      <c r="H5" s="204"/>
+      <c r="I5" s="204"/>
+      <c r="J5" s="204"/>
+      <c r="K5" s="204"/>
+      <c r="L5" s="204"/>
+      <c r="M5" s="204"/>
+      <c r="N5" s="204"/>
+      <c r="O5" s="204"/>
+      <c r="P5" s="204"/>
+      <c r="Q5" s="204"/>
+      <c r="R5" s="204"/>
+      <c r="S5" s="204"/>
+      <c r="T5" s="204"/>
       <c r="V5" s="3" t="s">
         <v>7</v>
       </c>
@@ -3170,24 +3464,24 @@
       <c r="B6" s="155" t="s">
         <v>424</v>
       </c>
-      <c r="C6" s="218"/>
-      <c r="D6" s="219"/>
-      <c r="E6" s="219"/>
-      <c r="F6" s="219"/>
-      <c r="G6" s="219"/>
-      <c r="H6" s="219"/>
-      <c r="I6" s="219"/>
-      <c r="J6" s="219"/>
-      <c r="K6" s="219"/>
-      <c r="L6" s="219"/>
-      <c r="M6" s="219"/>
-      <c r="N6" s="219"/>
-      <c r="O6" s="219"/>
-      <c r="P6" s="219"/>
-      <c r="Q6" s="219"/>
-      <c r="R6" s="219"/>
-      <c r="S6" s="219"/>
-      <c r="T6" s="219"/>
+      <c r="C6" s="188"/>
+      <c r="D6" s="204"/>
+      <c r="E6" s="204"/>
+      <c r="F6" s="204"/>
+      <c r="G6" s="204"/>
+      <c r="H6" s="204"/>
+      <c r="I6" s="204"/>
+      <c r="J6" s="204"/>
+      <c r="K6" s="204"/>
+      <c r="L6" s="204"/>
+      <c r="M6" s="204"/>
+      <c r="N6" s="204"/>
+      <c r="O6" s="204"/>
+      <c r="P6" s="204"/>
+      <c r="Q6" s="204"/>
+      <c r="R6" s="204"/>
+      <c r="S6" s="204"/>
+      <c r="T6" s="204"/>
       <c r="V6" s="3" t="s">
         <v>180</v>
       </c>
@@ -3199,151 +3493,151 @@
       <c r="B7" s="155" t="s">
         <v>425</v>
       </c>
-      <c r="C7" s="218"/>
-      <c r="D7" s="219"/>
-      <c r="E7" s="219"/>
-      <c r="F7" s="219"/>
-      <c r="G7" s="219"/>
-      <c r="H7" s="219"/>
-      <c r="I7" s="219"/>
-      <c r="J7" s="219"/>
-      <c r="K7" s="219"/>
-      <c r="L7" s="219"/>
-      <c r="M7" s="219"/>
-      <c r="N7" s="219"/>
-      <c r="O7" s="219"/>
-      <c r="P7" s="219"/>
-      <c r="Q7" s="219"/>
-      <c r="R7" s="219"/>
-      <c r="S7" s="219"/>
-      <c r="T7" s="219"/>
+      <c r="C7" s="188"/>
+      <c r="D7" s="204"/>
+      <c r="E7" s="204"/>
+      <c r="F7" s="204"/>
+      <c r="G7" s="204"/>
+      <c r="H7" s="204"/>
+      <c r="I7" s="204"/>
+      <c r="J7" s="204"/>
+      <c r="K7" s="204"/>
+      <c r="L7" s="204"/>
+      <c r="M7" s="204"/>
+      <c r="N7" s="204"/>
+      <c r="O7" s="204"/>
+      <c r="P7" s="204"/>
+      <c r="Q7" s="204"/>
+      <c r="R7" s="204"/>
+      <c r="S7" s="204"/>
+      <c r="T7" s="204"/>
     </row>
     <row r="8" spans="2:23" ht="15">
       <c r="B8" s="155" t="s">
         <v>426</v>
       </c>
-      <c r="C8" s="218"/>
-      <c r="D8" s="219"/>
-      <c r="E8" s="219"/>
-      <c r="F8" s="219"/>
-      <c r="G8" s="219"/>
-      <c r="H8" s="219"/>
-      <c r="I8" s="219"/>
-      <c r="J8" s="219"/>
-      <c r="K8" s="219"/>
-      <c r="L8" s="219"/>
-      <c r="M8" s="219"/>
-      <c r="N8" s="219"/>
-      <c r="O8" s="219"/>
-      <c r="P8" s="219"/>
-      <c r="Q8" s="219"/>
-      <c r="R8" s="219"/>
-      <c r="S8" s="219"/>
-      <c r="T8" s="219"/>
+      <c r="C8" s="188"/>
+      <c r="D8" s="204"/>
+      <c r="E8" s="204"/>
+      <c r="F8" s="204"/>
+      <c r="G8" s="204"/>
+      <c r="H8" s="204"/>
+      <c r="I8" s="204"/>
+      <c r="J8" s="204"/>
+      <c r="K8" s="204"/>
+      <c r="L8" s="204"/>
+      <c r="M8" s="204"/>
+      <c r="N8" s="204"/>
+      <c r="O8" s="204"/>
+      <c r="P8" s="204"/>
+      <c r="Q8" s="204"/>
+      <c r="R8" s="204"/>
+      <c r="S8" s="204"/>
+      <c r="T8" s="204"/>
     </row>
     <row r="9" spans="2:23" ht="15">
       <c r="B9" s="155" t="s">
         <v>427</v>
       </c>
-      <c r="C9" s="218"/>
-      <c r="D9" s="219"/>
-      <c r="E9" s="219"/>
-      <c r="F9" s="219"/>
-      <c r="G9" s="219"/>
-      <c r="H9" s="219"/>
-      <c r="I9" s="219"/>
-      <c r="J9" s="219"/>
-      <c r="K9" s="219"/>
-      <c r="L9" s="219"/>
-      <c r="M9" s="219"/>
-      <c r="N9" s="219"/>
-      <c r="O9" s="219"/>
-      <c r="P9" s="219"/>
-      <c r="Q9" s="219"/>
-      <c r="R9" s="219"/>
-      <c r="S9" s="219"/>
-      <c r="T9" s="219"/>
+      <c r="C9" s="188"/>
+      <c r="D9" s="204"/>
+      <c r="E9" s="204"/>
+      <c r="F9" s="204"/>
+      <c r="G9" s="204"/>
+      <c r="H9" s="204"/>
+      <c r="I9" s="204"/>
+      <c r="J9" s="204"/>
+      <c r="K9" s="204"/>
+      <c r="L9" s="204"/>
+      <c r="M9" s="204"/>
+      <c r="N9" s="204"/>
+      <c r="O9" s="204"/>
+      <c r="P9" s="204"/>
+      <c r="Q9" s="204"/>
+      <c r="R9" s="204"/>
+      <c r="S9" s="204"/>
+      <c r="T9" s="204"/>
     </row>
     <row r="10" spans="2:23" ht="15">
       <c r="B10" s="155" t="s">
         <v>428</v>
       </c>
-      <c r="C10" s="218"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="219"/>
-      <c r="H10" s="219"/>
-      <c r="I10" s="219"/>
-      <c r="J10" s="219"/>
-      <c r="K10" s="219"/>
-      <c r="L10" s="219"/>
-      <c r="M10" s="219"/>
-      <c r="N10" s="219"/>
-      <c r="O10" s="219"/>
-      <c r="P10" s="219"/>
-      <c r="Q10" s="219"/>
-      <c r="R10" s="219"/>
-      <c r="S10" s="219"/>
-      <c r="T10" s="219"/>
+      <c r="C10" s="188"/>
+      <c r="D10" s="204"/>
+      <c r="E10" s="204"/>
+      <c r="F10" s="204"/>
+      <c r="G10" s="204"/>
+      <c r="H10" s="204"/>
+      <c r="I10" s="204"/>
+      <c r="J10" s="204"/>
+      <c r="K10" s="204"/>
+      <c r="L10" s="204"/>
+      <c r="M10" s="204"/>
+      <c r="N10" s="204"/>
+      <c r="O10" s="204"/>
+      <c r="P10" s="204"/>
+      <c r="Q10" s="204"/>
+      <c r="R10" s="204"/>
+      <c r="S10" s="204"/>
+      <c r="T10" s="204"/>
     </row>
     <row r="11" spans="2:23" ht="15">
       <c r="B11" s="155" t="s">
         <v>429</v>
       </c>
-      <c r="C11" s="218"/>
-      <c r="D11" s="219"/>
-      <c r="E11" s="219"/>
-      <c r="F11" s="219"/>
-      <c r="G11" s="219"/>
-      <c r="H11" s="219"/>
-      <c r="I11" s="219"/>
-      <c r="J11" s="219"/>
-      <c r="K11" s="219"/>
-      <c r="L11" s="219"/>
-      <c r="M11" s="219"/>
-      <c r="N11" s="219"/>
-      <c r="O11" s="219"/>
-      <c r="P11" s="219"/>
-      <c r="Q11" s="219"/>
-      <c r="R11" s="219"/>
-      <c r="S11" s="219"/>
-      <c r="T11" s="219"/>
+      <c r="C11" s="188"/>
+      <c r="D11" s="204"/>
+      <c r="E11" s="204"/>
+      <c r="F11" s="204"/>
+      <c r="G11" s="204"/>
+      <c r="H11" s="204"/>
+      <c r="I11" s="204"/>
+      <c r="J11" s="204"/>
+      <c r="K11" s="204"/>
+      <c r="L11" s="204"/>
+      <c r="M11" s="204"/>
+      <c r="N11" s="204"/>
+      <c r="O11" s="204"/>
+      <c r="P11" s="204"/>
+      <c r="Q11" s="204"/>
+      <c r="R11" s="204"/>
+      <c r="S11" s="204"/>
+      <c r="T11" s="204"/>
     </row>
     <row r="12" spans="2:23" ht="15">
       <c r="B12" s="155" t="s">
         <v>430</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="219"/>
-      <c r="E12" s="219"/>
-      <c r="F12" s="219"/>
-      <c r="G12" s="219"/>
-      <c r="H12" s="219"/>
-      <c r="I12" s="219"/>
-      <c r="J12" s="219"/>
-      <c r="K12" s="219"/>
-      <c r="L12" s="219"/>
-      <c r="M12" s="219"/>
-      <c r="N12" s="219"/>
-      <c r="O12" s="219"/>
-      <c r="P12" s="219"/>
-      <c r="Q12" s="219"/>
-      <c r="R12" s="219"/>
-      <c r="S12" s="219"/>
-      <c r="T12" s="219"/>
+      <c r="D12" s="204"/>
+      <c r="E12" s="204"/>
+      <c r="F12" s="204"/>
+      <c r="G12" s="204"/>
+      <c r="H12" s="204"/>
+      <c r="I12" s="204"/>
+      <c r="J12" s="204"/>
+      <c r="K12" s="204"/>
+      <c r="L12" s="204"/>
+      <c r="M12" s="204"/>
+      <c r="N12" s="204"/>
+      <c r="O12" s="204"/>
+      <c r="P12" s="204"/>
+      <c r="Q12" s="204"/>
+      <c r="R12" s="204"/>
+      <c r="S12" s="204"/>
+      <c r="T12" s="204"/>
     </row>
     <row r="13" spans="2:23" ht="13"/>
     <row r="14" spans="2:23" ht="15">
-      <c r="B14" s="188" t="s">
+      <c r="B14" s="200" t="s">
         <v>435</v>
       </c>
-      <c r="C14" s="189"/>
-      <c r="E14" s="190" t="s">
+      <c r="C14" s="201"/>
+      <c r="E14" s="202" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="221"/>
-      <c r="G14" s="221"/>
+      <c r="F14" s="203"/>
+      <c r="G14" s="203"/>
     </row>
     <row r="15" spans="2:23" ht="15">
       <c r="B15" s="155" t="s">
@@ -3372,7 +3666,7 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="15">
-      <c r="B17" s="220" t="s">
+      <c r="B17" s="155" t="s">
         <v>95</v>
       </c>
       <c r="C17" s="2"/>
@@ -3387,7 +3681,7 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="15">
-      <c r="B18" s="220" t="s">
+      <c r="B18" s="155" t="s">
         <v>92</v>
       </c>
       <c r="C18" s="2"/>
@@ -3400,7 +3694,7 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="15">
-      <c r="B19" s="220" t="s">
+      <c r="B19" s="155" t="s">
         <v>437</v>
       </c>
       <c r="C19" s="2"/>
@@ -3416,7 +3710,7 @@
       </c>
     </row>
     <row r="20" spans="2:8" ht="15">
-      <c r="B20" s="220" t="s">
+      <c r="B20" s="155" t="s">
         <v>438</v>
       </c>
       <c r="C20" s="2"/>
@@ -3642,6 +3936,652 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A88C279-C091-A94C-B283-276290F6C98F}">
+  <dimension ref="A2:H49"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="8" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="14" customHeight="1">
+      <c r="B2" s="227" t="s">
+        <v>440</v>
+      </c>
+      <c r="C2" s="236"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
+      <c r="F2" s="236"/>
+      <c r="G2" s="236"/>
+      <c r="H2" s="236"/>
+    </row>
+    <row r="3" spans="2:8" ht="13" customHeight="1">
+      <c r="B3" s="237"/>
+      <c r="C3" s="238"/>
+      <c r="D3" s="238"/>
+      <c r="E3" s="238"/>
+      <c r="F3" s="238"/>
+      <c r="G3" s="238"/>
+      <c r="H3" s="238"/>
+    </row>
+    <row r="4" spans="2:8" ht="16" customHeight="1">
+      <c r="B4" s="191" t="s">
+        <v>441</v>
+      </c>
+      <c r="C4" s="239" t="s">
+        <v>468</v>
+      </c>
+      <c r="D4" s="240"/>
+      <c r="E4" s="239" t="s">
+        <v>469</v>
+      </c>
+      <c r="F4" s="240"/>
+      <c r="G4" s="196" t="s">
+        <v>470</v>
+      </c>
+      <c r="H4" s="196" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="15">
+      <c r="B5" s="192"/>
+      <c r="C5" s="196"/>
+      <c r="D5" s="196"/>
+      <c r="E5" s="196"/>
+      <c r="F5" s="196"/>
+      <c r="G5" s="196"/>
+      <c r="H5" s="196"/>
+    </row>
+    <row r="6" spans="2:8" ht="15">
+      <c r="B6" s="135" t="s">
+        <v>446</v>
+      </c>
+      <c r="C6" s="234"/>
+      <c r="D6" s="234"/>
+      <c r="E6" s="234"/>
+      <c r="F6" s="234"/>
+      <c r="G6" s="148"/>
+      <c r="H6" s="148"/>
+    </row>
+    <row r="7" spans="2:8" ht="15">
+      <c r="B7" s="135" t="s">
+        <v>445</v>
+      </c>
+      <c r="C7" s="229"/>
+      <c r="D7" s="229"/>
+      <c r="E7" s="229"/>
+      <c r="F7" s="229"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="147"/>
+    </row>
+    <row r="8" spans="2:8" ht="15">
+      <c r="B8" s="135" t="s">
+        <v>444</v>
+      </c>
+      <c r="C8" s="229"/>
+      <c r="D8" s="229"/>
+      <c r="E8" s="229"/>
+      <c r="F8" s="229"/>
+      <c r="G8" s="147"/>
+      <c r="H8" s="147"/>
+    </row>
+    <row r="9" spans="2:8" ht="15">
+      <c r="B9" s="135" t="s">
+        <v>443</v>
+      </c>
+      <c r="C9" s="229"/>
+      <c r="D9" s="229"/>
+      <c r="E9" s="229"/>
+      <c r="F9" s="229"/>
+      <c r="G9" s="147"/>
+      <c r="H9" s="147"/>
+    </row>
+    <row r="10" spans="2:8" ht="15">
+      <c r="B10" s="135" t="s">
+        <v>442</v>
+      </c>
+      <c r="C10" s="229"/>
+      <c r="D10" s="229"/>
+      <c r="E10" s="229"/>
+      <c r="F10" s="229"/>
+      <c r="G10" s="147"/>
+      <c r="H10" s="147"/>
+    </row>
+    <row r="11" spans="2:8" ht="15">
+      <c r="B11" s="135"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
+      <c r="H11" s="136"/>
+    </row>
+    <row r="12" spans="2:8" ht="15">
+      <c r="B12" s="193" t="s">
+        <v>447</v>
+      </c>
+      <c r="C12" s="232" t="s">
+        <v>468</v>
+      </c>
+      <c r="D12" s="233"/>
+      <c r="E12" s="232" t="s">
+        <v>469</v>
+      </c>
+      <c r="F12" s="233"/>
+      <c r="G12" s="195" t="s">
+        <v>470</v>
+      </c>
+      <c r="H12" s="195" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="15">
+      <c r="B13" s="194"/>
+      <c r="C13" s="196"/>
+      <c r="D13" s="196"/>
+      <c r="E13" s="196"/>
+      <c r="F13" s="196"/>
+      <c r="G13" s="196"/>
+      <c r="H13" s="196"/>
+    </row>
+    <row r="14" spans="2:8" ht="15">
+      <c r="B14" s="135" t="s">
+        <v>446</v>
+      </c>
+      <c r="C14" s="234"/>
+      <c r="D14" s="234"/>
+      <c r="E14" s="234"/>
+      <c r="F14" s="234"/>
+      <c r="G14" s="148"/>
+      <c r="H14" s="148"/>
+    </row>
+    <row r="15" spans="2:8" ht="15">
+      <c r="B15" s="135" t="s">
+        <v>445</v>
+      </c>
+      <c r="C15" s="235"/>
+      <c r="D15" s="235"/>
+      <c r="E15" s="235"/>
+      <c r="F15" s="235"/>
+      <c r="G15" s="148"/>
+      <c r="H15" s="148"/>
+    </row>
+    <row r="16" spans="2:8" ht="15">
+      <c r="B16" s="135" t="s">
+        <v>444</v>
+      </c>
+      <c r="C16" s="235"/>
+      <c r="D16" s="235"/>
+      <c r="E16" s="235"/>
+      <c r="F16" s="235"/>
+      <c r="G16" s="148"/>
+      <c r="H16" s="148"/>
+    </row>
+    <row r="17" spans="1:8" ht="15">
+      <c r="B17" s="135" t="s">
+        <v>443</v>
+      </c>
+      <c r="C17" s="235"/>
+      <c r="D17" s="235"/>
+      <c r="E17" s="235"/>
+      <c r="F17" s="235"/>
+      <c r="G17" s="148"/>
+      <c r="H17" s="148"/>
+    </row>
+    <row r="18" spans="1:8" ht="15">
+      <c r="B18" s="135" t="s">
+        <v>448</v>
+      </c>
+      <c r="C18" s="235"/>
+      <c r="D18" s="235"/>
+      <c r="E18" s="235"/>
+      <c r="F18" s="235"/>
+      <c r="G18" s="148"/>
+      <c r="H18" s="148"/>
+    </row>
+    <row r="19" spans="1:8" ht="15">
+      <c r="B19" s="135" t="s">
+        <v>449</v>
+      </c>
+      <c r="C19" s="235"/>
+      <c r="D19" s="235"/>
+      <c r="E19" s="235"/>
+      <c r="F19" s="235"/>
+      <c r="G19" s="148"/>
+      <c r="H19" s="148"/>
+    </row>
+    <row r="20" spans="1:8" ht="15">
+      <c r="C20" s="136"/>
+      <c r="D20" s="136"/>
+      <c r="E20" s="136"/>
+      <c r="F20" s="136"/>
+      <c r="G20" s="136"/>
+      <c r="H20" s="136"/>
+    </row>
+    <row r="21" spans="1:8" ht="15">
+      <c r="B21" s="137" t="s">
+        <v>450</v>
+      </c>
+      <c r="C21" s="232"/>
+      <c r="D21" s="233"/>
+      <c r="E21" s="232"/>
+      <c r="F21" s="233"/>
+      <c r="G21" s="195"/>
+      <c r="H21" s="195"/>
+    </row>
+    <row r="22" spans="1:8" ht="15">
+      <c r="B22" s="135" t="s">
+        <v>451</v>
+      </c>
+      <c r="C22" s="241"/>
+      <c r="D22" s="241"/>
+      <c r="E22" s="241"/>
+      <c r="F22" s="241"/>
+      <c r="G22" s="147"/>
+      <c r="H22" s="147"/>
+    </row>
+    <row r="23" spans="1:8" ht="15">
+      <c r="B23" s="135" t="s">
+        <v>452</v>
+      </c>
+      <c r="C23" s="229"/>
+      <c r="D23" s="229"/>
+      <c r="E23" s="229"/>
+      <c r="F23" s="229"/>
+      <c r="G23" s="147"/>
+      <c r="H23" s="147"/>
+    </row>
+    <row r="24" spans="1:8" ht="15">
+      <c r="B24" s="135" t="s">
+        <v>453</v>
+      </c>
+      <c r="C24" s="229"/>
+      <c r="D24" s="229"/>
+      <c r="E24" s="229"/>
+      <c r="F24" s="229"/>
+      <c r="G24" s="147"/>
+      <c r="H24" s="147"/>
+    </row>
+    <row r="25" spans="1:8" ht="15">
+      <c r="B25" s="135" t="s">
+        <v>454</v>
+      </c>
+      <c r="C25" s="229"/>
+      <c r="D25" s="229"/>
+      <c r="E25" s="229"/>
+      <c r="F25" s="229"/>
+      <c r="G25" s="147"/>
+      <c r="H25" s="147"/>
+    </row>
+    <row r="26" spans="1:8" ht="15">
+      <c r="B26" s="135" t="s">
+        <v>455</v>
+      </c>
+      <c r="C26" s="229"/>
+      <c r="D26" s="229"/>
+      <c r="E26" s="229"/>
+      <c r="F26" s="229"/>
+      <c r="G26" s="199"/>
+      <c r="H26" s="199"/>
+    </row>
+    <row r="27" spans="1:8" ht="15">
+      <c r="B27" s="135" t="s">
+        <v>456</v>
+      </c>
+      <c r="C27" s="229"/>
+      <c r="D27" s="229"/>
+      <c r="E27" s="229"/>
+      <c r="F27" s="229"/>
+      <c r="G27" s="199"/>
+      <c r="H27" s="199"/>
+    </row>
+    <row r="28" spans="1:8" ht="15">
+      <c r="A28" s="155"/>
+      <c r="C28" s="186"/>
+      <c r="D28" s="186"/>
+      <c r="E28" s="186"/>
+      <c r="F28" s="186"/>
+      <c r="G28" s="186"/>
+      <c r="H28" s="186"/>
+    </row>
+    <row r="29" spans="1:8" ht="15">
+      <c r="A29" s="155"/>
+      <c r="B29" s="189" t="s">
+        <v>467</v>
+      </c>
+      <c r="C29" s="232" t="s">
+        <v>468</v>
+      </c>
+      <c r="D29" s="233"/>
+      <c r="E29" s="232" t="s">
+        <v>469</v>
+      </c>
+      <c r="F29" s="233"/>
+      <c r="G29" s="195" t="s">
+        <v>470</v>
+      </c>
+      <c r="H29" s="195" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15">
+      <c r="A30" s="155"/>
+      <c r="B30" s="190"/>
+      <c r="C30" s="196"/>
+      <c r="D30" s="196"/>
+      <c r="E30" s="196"/>
+      <c r="F30" s="196"/>
+      <c r="G30" s="196"/>
+      <c r="H30" s="196"/>
+    </row>
+    <row r="31" spans="1:8" ht="15">
+      <c r="A31" s="155"/>
+      <c r="B31" s="153" t="s">
+        <v>472</v>
+      </c>
+      <c r="C31" s="230"/>
+      <c r="D31" s="230"/>
+      <c r="E31" s="230"/>
+      <c r="F31" s="230"/>
+      <c r="G31" s="197"/>
+      <c r="H31" s="197"/>
+    </row>
+    <row r="32" spans="1:8" ht="15">
+      <c r="A32" s="155"/>
+      <c r="B32" s="153" t="s">
+        <v>473</v>
+      </c>
+      <c r="C32" s="229"/>
+      <c r="D32" s="229"/>
+      <c r="E32" s="229"/>
+      <c r="F32" s="229"/>
+      <c r="G32" s="197"/>
+      <c r="H32" s="197"/>
+    </row>
+    <row r="33" spans="1:8" ht="15">
+      <c r="A33" s="155"/>
+      <c r="B33" s="153" t="s">
+        <v>474</v>
+      </c>
+      <c r="C33" s="229"/>
+      <c r="D33" s="229"/>
+      <c r="E33" s="229"/>
+      <c r="F33" s="229"/>
+      <c r="G33" s="197"/>
+      <c r="H33" s="197"/>
+    </row>
+    <row r="34" spans="1:8" ht="15">
+      <c r="A34" s="155"/>
+      <c r="B34" s="153" t="s">
+        <v>475</v>
+      </c>
+      <c r="C34" s="229"/>
+      <c r="D34" s="229"/>
+      <c r="E34" s="229"/>
+      <c r="F34" s="229"/>
+      <c r="G34" s="197"/>
+      <c r="H34" s="197"/>
+    </row>
+    <row r="35" spans="1:8" ht="15">
+      <c r="A35" s="155"/>
+      <c r="B35" s="153" t="s">
+        <v>476</v>
+      </c>
+      <c r="C35" s="229"/>
+      <c r="D35" s="229"/>
+      <c r="E35" s="229"/>
+      <c r="F35" s="229"/>
+      <c r="G35" s="197"/>
+      <c r="H35" s="197"/>
+    </row>
+    <row r="36" spans="1:8" ht="15">
+      <c r="B36" s="135"/>
+      <c r="C36" s="186"/>
+      <c r="D36" s="186"/>
+      <c r="E36" s="186"/>
+      <c r="F36" s="186"/>
+      <c r="G36" s="186"/>
+      <c r="H36" s="186"/>
+    </row>
+    <row r="37" spans="1:8" ht="15">
+      <c r="A37" s="155"/>
+      <c r="B37" s="185" t="s">
+        <v>457</v>
+      </c>
+      <c r="C37" s="242"/>
+      <c r="D37" s="243"/>
+      <c r="E37" s="242"/>
+      <c r="F37" s="243"/>
+      <c r="G37" s="198"/>
+      <c r="H37" s="198"/>
+    </row>
+    <row r="38" spans="1:8" ht="15">
+      <c r="B38" s="135" t="s">
+        <v>458</v>
+      </c>
+      <c r="C38" s="241"/>
+      <c r="D38" s="241"/>
+      <c r="E38" s="241"/>
+      <c r="F38" s="241"/>
+      <c r="G38" s="147"/>
+      <c r="H38" s="147"/>
+    </row>
+    <row r="39" spans="1:8" ht="15">
+      <c r="B39" s="135" t="s">
+        <v>459</v>
+      </c>
+      <c r="C39" s="229"/>
+      <c r="D39" s="229"/>
+      <c r="E39" s="229"/>
+      <c r="F39" s="229"/>
+      <c r="G39" s="147"/>
+      <c r="H39" s="147"/>
+    </row>
+    <row r="40" spans="1:8" ht="15">
+      <c r="B40" s="135" t="s">
+        <v>460</v>
+      </c>
+      <c r="C40" s="229"/>
+      <c r="D40" s="229"/>
+      <c r="E40" s="229"/>
+      <c r="F40" s="229"/>
+      <c r="G40" s="147"/>
+      <c r="H40" s="147"/>
+    </row>
+    <row r="41" spans="1:8" ht="15">
+      <c r="B41" s="135" t="s">
+        <v>461</v>
+      </c>
+      <c r="C41" s="229"/>
+      <c r="D41" s="229"/>
+      <c r="E41" s="229"/>
+      <c r="F41" s="229"/>
+      <c r="G41" s="147"/>
+      <c r="H41" s="147"/>
+    </row>
+    <row r="42" spans="1:8" ht="15">
+      <c r="B42" s="135"/>
+      <c r="C42" s="136"/>
+      <c r="D42" s="136"/>
+      <c r="E42" s="136"/>
+      <c r="F42" s="136"/>
+      <c r="G42" s="136"/>
+      <c r="H42" s="136"/>
+    </row>
+    <row r="43" spans="1:8" ht="15">
+      <c r="A43" s="155"/>
+      <c r="B43" s="189" t="s">
+        <v>462</v>
+      </c>
+      <c r="C43" s="232" t="s">
+        <v>468</v>
+      </c>
+      <c r="D43" s="233"/>
+      <c r="E43" s="232" t="s">
+        <v>469</v>
+      </c>
+      <c r="F43" s="233"/>
+      <c r="G43" s="195" t="s">
+        <v>470</v>
+      </c>
+      <c r="H43" s="195" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15">
+      <c r="A44" s="155"/>
+      <c r="B44" s="190"/>
+      <c r="C44" s="196"/>
+      <c r="D44" s="196"/>
+      <c r="E44" s="196"/>
+      <c r="F44" s="196"/>
+      <c r="G44" s="196"/>
+      <c r="H44" s="196"/>
+    </row>
+    <row r="45" spans="1:8" ht="15">
+      <c r="A45" s="155"/>
+      <c r="B45" s="153" t="s">
+        <v>463</v>
+      </c>
+      <c r="C45" s="230"/>
+      <c r="D45" s="230"/>
+      <c r="E45" s="230"/>
+      <c r="F45" s="230"/>
+      <c r="G45" s="197"/>
+      <c r="H45" s="197"/>
+    </row>
+    <row r="46" spans="1:8" ht="15">
+      <c r="A46" s="155"/>
+      <c r="B46" s="153" t="s">
+        <v>464</v>
+      </c>
+      <c r="C46" s="231"/>
+      <c r="D46" s="231"/>
+      <c r="E46" s="231"/>
+      <c r="F46" s="231"/>
+      <c r="G46" s="197"/>
+      <c r="H46" s="197"/>
+    </row>
+    <row r="47" spans="1:8" ht="15">
+      <c r="A47" s="155"/>
+      <c r="B47" s="153" t="s">
+        <v>465</v>
+      </c>
+      <c r="C47" s="231"/>
+      <c r="D47" s="231"/>
+      <c r="E47" s="231"/>
+      <c r="F47" s="231"/>
+      <c r="G47" s="197"/>
+      <c r="H47" s="197"/>
+    </row>
+    <row r="48" spans="1:8" ht="15">
+      <c r="A48" s="155"/>
+      <c r="B48" s="153" t="s">
+        <v>466</v>
+      </c>
+      <c r="C48" s="231"/>
+      <c r="D48" s="231"/>
+      <c r="E48" s="231"/>
+      <c r="F48" s="231"/>
+      <c r="G48" s="197"/>
+      <c r="H48" s="197"/>
+    </row>
+    <row r="49" spans="3:8" ht="15">
+      <c r="C49" s="136"/>
+      <c r="D49" s="136"/>
+      <c r="E49" s="136"/>
+      <c r="F49" s="136"/>
+      <c r="G49" s="136"/>
+      <c r="H49" s="136"/>
+    </row>
+  </sheetData>
+  <mergeCells count="73">
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{183A8D03-1BB5-B745-9DC6-FDA2F464E650}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="B2:O47"/>
@@ -3657,7 +4597,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15">
-      <c r="B2" s="216" t="s">
+      <c r="B2" s="244" t="s">
         <v>224</v>
       </c>
       <c r="C2" s="175" t="s">
@@ -3701,7 +4641,7 @@
       </c>
     </row>
     <row r="3" spans="2:15" ht="14">
-      <c r="B3" s="217"/>
+      <c r="B3" s="245"/>
       <c r="C3" s="176">
         <v>40446</v>
       </c>
@@ -5316,11 +6256,11 @@
     </row>
     <row r="2" spans="1:24" ht="21">
       <c r="A2" s="8"/>
-      <c r="B2" s="198" t="str">
+      <c r="B2" s="211" t="str">
         <f>CONCATENATE(INFO!C4, " ", "DCF")</f>
         <v xml:space="preserve"> DCF</v>
       </c>
-      <c r="C2" s="199"/>
+      <c r="C2" s="212"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -5381,10 +6321,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="192" t="s">
+      <c r="E4" s="205" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="193"/>
+      <c r="F4" s="206"/>
       <c r="G4" s="11" t="e">
         <f ca="1">Z88</f>
         <v>#REF!</v>
@@ -5418,13 +6358,13 @@
       </c>
       <c r="C5" s="13">
         <f ca="1">TODAY()</f>
-        <v>45319</v>
+        <v>45330</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="192" t="s">
+      <c r="E5" s="205" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="193"/>
+      <c r="F5" s="206"/>
       <c r="G5" s="14" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -5484,10 +6424,10 @@
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="196" t="s">
+      <c r="B7" s="209" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="200"/>
+      <c r="C7" s="213"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -5518,10 +6458,10 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="197" t="s">
+      <c r="F8" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="193"/>
+      <c r="G8" s="206"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="10" t="s">
@@ -5530,10 +6470,10 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="197" t="s">
+      <c r="N8" s="210" t="s">
         <v>43</v>
       </c>
-      <c r="O8" s="193"/>
+      <c r="O8" s="206"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -5546,19 +6486,19 @@
     </row>
     <row r="9" spans="1:24" ht="15">
       <c r="A9" s="1"/>
-      <c r="B9" s="192" t="s">
+      <c r="B9" s="205" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="193"/>
+      <c r="C9" s="206"/>
       <c r="D9" s="2">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="192" t="e">
+      <c r="F9" s="205" t="e">
         <f>CONCATENATE("Revenue", " ",Q43)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G9" s="193"/>
+      <c r="G9" s="206"/>
       <c r="H9" s="2" t="e">
         <f>Q47-1%</f>
         <v>#REF!</v>
@@ -5568,11 +6508,11 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="192" t="e">
+      <c r="N9" s="205" t="e">
         <f>CONCATENATE("Revenue ", Q43)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O9" s="193"/>
+      <c r="O9" s="206"/>
       <c r="P9" s="2" t="e">
         <f>Q47+1%</f>
         <v>#REF!</v>
@@ -5587,37 +6527,37 @@
     </row>
     <row r="10" spans="1:24" ht="15">
       <c r="A10" s="1"/>
-      <c r="B10" s="192" t="s">
+      <c r="B10" s="205" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="193"/>
+      <c r="C10" s="206"/>
       <c r="D10" s="16">
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="192" t="e">
+      <c r="F10" s="205" t="e">
         <f>CONCATENATE("Revenue ", Z43)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G10" s="193"/>
+      <c r="G10" s="206"/>
       <c r="H10" s="17">
         <v>0.03</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="192" t="e">
+      <c r="J10" s="205" t="e">
         <f>CONCATENATE("Revenue ", Z43)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K10" s="193"/>
+      <c r="K10" s="206"/>
       <c r="L10" s="18">
         <v>0.05</v>
       </c>
       <c r="M10" s="1"/>
-      <c r="N10" s="192" t="e">
+      <c r="N10" s="205" t="e">
         <f>CONCATENATE("Revenue ", Z43)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O10" s="193"/>
+      <c r="O10" s="206"/>
       <c r="P10" s="17">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -5768,20 +6708,20 @@
         <v>0.09</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="192" t="e">
+      <c r="J14" s="205" t="e">
         <f>CONCATENATE("CapEx ", Z43)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K14" s="193"/>
+      <c r="K14" s="206"/>
       <c r="L14" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="M14" s="1"/>
-      <c r="N14" s="192" t="e">
+      <c r="N14" s="205" t="e">
         <f>CONCATENATE("CapEx ", Z43)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O14" s="193"/>
+      <c r="O14" s="206"/>
       <c r="P14" s="17">
         <v>0.05</v>
       </c>
@@ -5874,10 +6814,10 @@
     </row>
     <row r="17" spans="1:24" ht="15">
       <c r="A17" s="1"/>
-      <c r="B17" s="197" t="s">
+      <c r="B17" s="210" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="193"/>
+      <c r="C17" s="206"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -5992,10 +6932,10 @@
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="196" t="s">
+      <c r="B21" s="209" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="193"/>
+      <c r="C21" s="206"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="19" t="str">
@@ -6292,10 +7232,10 @@
     </row>
     <row r="26" spans="1:24" ht="15">
       <c r="A26" s="1"/>
-      <c r="B26" s="195" t="s">
+      <c r="B26" s="208" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="193"/>
+      <c r="C26" s="206"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="24" t="e">
@@ -6525,10 +7465,10 @@
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="196" t="s">
+      <c r="B31" s="209" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="193"/>
+      <c r="C31" s="206"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="19" t="str">
@@ -6672,10 +7612,10 @@
     </row>
     <row r="33" spans="1:26" ht="15">
       <c r="A33" s="1"/>
-      <c r="B33" s="195" t="s">
+      <c r="B33" s="208" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="193"/>
+      <c r="C33" s="206"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="24" t="e">
@@ -6742,10 +7682,10 @@
     </row>
     <row r="34" spans="1:26" ht="15">
       <c r="A34" s="1"/>
-      <c r="B34" s="195" t="s">
+      <c r="B34" s="208" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="193"/>
+      <c r="C34" s="206"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="24" t="e">
@@ -6824,10 +7764,10 @@
     </row>
     <row r="36" spans="1:26" ht="15">
       <c r="A36" s="1"/>
-      <c r="B36" s="192" t="s">
+      <c r="B36" s="205" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="193"/>
+      <c r="C36" s="206"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="20">
@@ -6894,10 +7834,10 @@
     </row>
     <row r="37" spans="1:26" ht="15">
       <c r="A37" s="1"/>
-      <c r="B37" s="195" t="s">
+      <c r="B37" s="208" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="193"/>
+      <c r="C37" s="206"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="24" t="e">
@@ -6991,10 +7931,10 @@
     </row>
     <row r="39" spans="1:26" ht="15">
       <c r="A39" s="1"/>
-      <c r="B39" s="192" t="s">
+      <c r="B39" s="205" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="193"/>
+      <c r="C39" s="206"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="32">
@@ -7054,10 +7994,10 @@
     </row>
     <row r="40" spans="1:26" ht="15">
       <c r="A40" s="1"/>
-      <c r="B40" s="195" t="s">
+      <c r="B40" s="208" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="193"/>
+      <c r="C40" s="206"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="24" t="e">
@@ -7117,10 +8057,10 @@
     </row>
     <row r="41" spans="1:26" ht="15">
       <c r="A41" s="1"/>
-      <c r="B41" s="195" t="s">
+      <c r="B41" s="208" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="193"/>
+      <c r="C41" s="206"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="23"/>
@@ -7493,10 +8433,10 @@
     </row>
     <row r="46" spans="1:26" ht="15">
       <c r="A46" s="1"/>
-      <c r="B46" s="192" t="s">
+      <c r="B46" s="205" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="193"/>
+      <c r="C46" s="206"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -7550,11 +8490,11 @@
     </row>
     <row r="47" spans="1:26" ht="15">
       <c r="A47" s="1"/>
-      <c r="B47" s="192" t="s">
+      <c r="B47" s="205" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="193"/>
-      <c r="D47" s="193"/>
+      <c r="C47" s="206"/>
+      <c r="D47" s="206"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -7607,10 +8547,10 @@
     </row>
     <row r="48" spans="1:26" ht="15">
       <c r="A48" s="1"/>
-      <c r="B48" s="192" t="s">
+      <c r="B48" s="205" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="193"/>
+      <c r="C48" s="206"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -7875,10 +8815,10 @@
     </row>
     <row r="52" spans="1:26" ht="15">
       <c r="A52" s="1"/>
-      <c r="B52" s="192" t="s">
+      <c r="B52" s="205" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="193"/>
+      <c r="C52" s="206"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -7932,11 +8872,11 @@
     </row>
     <row r="53" spans="1:26" ht="15">
       <c r="A53" s="1"/>
-      <c r="B53" s="192" t="s">
+      <c r="B53" s="205" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="193"/>
-      <c r="D53" s="193"/>
+      <c r="C53" s="206"/>
+      <c r="D53" s="206"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -7989,10 +8929,10 @@
     </row>
     <row r="54" spans="1:26" ht="15">
       <c r="A54" s="1"/>
-      <c r="B54" s="192" t="s">
+      <c r="B54" s="205" t="s">
         <v>43</v>
       </c>
-      <c r="C54" s="193"/>
+      <c r="C54" s="206"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -8257,10 +9197,10 @@
     </row>
     <row r="58" spans="1:26" ht="15">
       <c r="A58" s="1"/>
-      <c r="B58" s="192" t="s">
+      <c r="B58" s="205" t="s">
         <v>41</v>
       </c>
-      <c r="C58" s="193"/>
+      <c r="C58" s="206"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -8314,11 +9254,11 @@
     </row>
     <row r="59" spans="1:26" ht="15">
       <c r="A59" s="1"/>
-      <c r="B59" s="192" t="s">
+      <c r="B59" s="205" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="193"/>
-      <c r="D59" s="193"/>
+      <c r="C59" s="206"/>
+      <c r="D59" s="206"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -8371,10 +9311,10 @@
     </row>
     <row r="60" spans="1:26" ht="15">
       <c r="A60" s="1"/>
-      <c r="B60" s="192" t="s">
+      <c r="B60" s="205" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="193"/>
+      <c r="C60" s="206"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -8730,10 +9670,10 @@
     </row>
     <row r="66" spans="1:28" ht="15">
       <c r="A66" s="1"/>
-      <c r="B66" s="192" t="s">
+      <c r="B66" s="205" t="s">
         <v>41</v>
       </c>
-      <c r="C66" s="193"/>
+      <c r="C66" s="206"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -8790,11 +9730,11 @@
     </row>
     <row r="67" spans="1:28" ht="15">
       <c r="A67" s="1"/>
-      <c r="B67" s="192" t="s">
+      <c r="B67" s="205" t="s">
         <v>65</v>
       </c>
-      <c r="C67" s="193"/>
-      <c r="D67" s="193"/>
+      <c r="C67" s="206"/>
+      <c r="D67" s="206"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -8850,10 +9790,10 @@
     </row>
     <row r="68" spans="1:28" ht="15">
       <c r="A68" s="1"/>
-      <c r="B68" s="192" t="s">
+      <c r="B68" s="205" t="s">
         <v>43</v>
       </c>
-      <c r="C68" s="193"/>
+      <c r="C68" s="206"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -9127,10 +10067,10 @@
     </row>
     <row r="72" spans="1:28" ht="15">
       <c r="A72" s="1"/>
-      <c r="B72" s="192" t="s">
+      <c r="B72" s="205" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="193"/>
+      <c r="C72" s="206"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -9191,11 +10131,11 @@
     </row>
     <row r="73" spans="1:28" ht="15">
       <c r="A73" s="1"/>
-      <c r="B73" s="192" t="s">
+      <c r="B73" s="205" t="s">
         <v>65</v>
       </c>
-      <c r="C73" s="193"/>
-      <c r="D73" s="193"/>
+      <c r="C73" s="206"/>
+      <c r="D73" s="206"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -9251,10 +10191,10 @@
     </row>
     <row r="74" spans="1:28" ht="15">
       <c r="A74" s="1"/>
-      <c r="B74" s="192" t="s">
+      <c r="B74" s="205" t="s">
         <v>43</v>
       </c>
-      <c r="C74" s="193"/>
+      <c r="C74" s="206"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -9342,10 +10282,10 @@
     </row>
     <row r="76" spans="1:28" ht="15">
       <c r="A76" s="1"/>
-      <c r="B76" s="192" t="s">
+      <c r="B76" s="205" t="s">
         <v>63</v>
       </c>
-      <c r="C76" s="193"/>
+      <c r="C76" s="206"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="32">
@@ -9556,11 +10496,11 @@
     </row>
     <row r="79" spans="1:28" ht="15">
       <c r="A79" s="1"/>
-      <c r="B79" s="194" t="s">
+      <c r="B79" s="207" t="s">
         <v>70</v>
       </c>
-      <c r="C79" s="193"/>
-      <c r="D79" s="193"/>
+      <c r="C79" s="206"/>
+      <c r="D79" s="206"/>
       <c r="E79" s="61"/>
       <c r="F79" s="61"/>
       <c r="G79" s="61"/>
@@ -9616,11 +10556,11 @@
     </row>
     <row r="80" spans="1:28" ht="15">
       <c r="A80" s="1"/>
-      <c r="B80" s="192" t="s">
+      <c r="B80" s="205" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="193"/>
-      <c r="D80" s="193"/>
+      <c r="C80" s="206"/>
+      <c r="D80" s="206"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -9672,10 +10612,10 @@
     </row>
     <row r="81" spans="1:26" ht="15">
       <c r="A81" s="1"/>
-      <c r="B81" s="192" t="s">
+      <c r="B81" s="205" t="s">
         <v>72</v>
       </c>
-      <c r="C81" s="193"/>
+      <c r="C81" s="206"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
@@ -9704,11 +10644,11 @@
     </row>
     <row r="82" spans="1:26" ht="15">
       <c r="A82" s="1"/>
-      <c r="B82" s="192" t="s">
+      <c r="B82" s="205" t="s">
         <v>73</v>
       </c>
-      <c r="C82" s="193"/>
-      <c r="D82" s="193"/>
+      <c r="C82" s="206"/>
+      <c r="D82" s="206"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
@@ -9736,10 +10676,10 @@
     </row>
     <row r="83" spans="1:26" ht="15">
       <c r="A83" s="1"/>
-      <c r="B83" s="192" t="s">
+      <c r="B83" s="205" t="s">
         <v>74</v>
       </c>
-      <c r="C83" s="193"/>
+      <c r="C83" s="206"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
@@ -9832,10 +10772,10 @@
     </row>
     <row r="86" spans="1:26" ht="15">
       <c r="A86" s="1"/>
-      <c r="B86" s="192" t="s">
+      <c r="B86" s="205" t="s">
         <v>77</v>
       </c>
-      <c r="C86" s="193"/>
+      <c r="C86" s="206"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -9864,10 +10804,10 @@
     </row>
     <row r="87" spans="1:26" ht="15">
       <c r="A87" s="1"/>
-      <c r="B87" s="192" t="s">
+      <c r="B87" s="205" t="s">
         <v>78</v>
       </c>
-      <c r="C87" s="193"/>
+      <c r="C87" s="206"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -9896,10 +10836,10 @@
     </row>
     <row r="88" spans="1:26" ht="15">
       <c r="A88" s="1"/>
-      <c r="B88" s="192" t="s">
+      <c r="B88" s="205" t="s">
         <v>79</v>
       </c>
-      <c r="C88" s="193"/>
+      <c r="C88" s="206"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -10006,29 +10946,29 @@
     <mergeCell ref="B88:C88"/>
   </mergeCells>
   <conditionalFormatting sqref="F76:P76">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:L5">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="greaterThan">
+      <formula>"0%"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="greaterThan">
       <formula>"10%"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThanOrEqual">
-      <formula>"0%"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="lessThanOrEqual">
       <formula>"0%"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T21:T22 F22:S22 F25:T25 F28:P28 T31 F32:P32 F36:P36 F39:P39">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10043,7 +10983,7 @@
   </sheetPr>
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -10126,29 +11066,29 @@
     </row>
     <row r="5" spans="1:26" ht="15">
       <c r="A5" s="1"/>
-      <c r="B5" s="197" t="s">
+      <c r="B5" s="210" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="193"/>
-      <c r="D5" s="193"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="193"/>
-      <c r="G5" s="193"/>
+      <c r="C5" s="206"/>
+      <c r="D5" s="206"/>
+      <c r="E5" s="206"/>
+      <c r="F5" s="206"/>
+      <c r="G5" s="206"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="15">
       <c r="A6" s="1"/>
-      <c r="B6" s="197" t="s">
+      <c r="B6" s="210" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="193"/>
-      <c r="D6" s="193"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="193"/>
-      <c r="G6" s="193"/>
-      <c r="H6" s="193"/>
+      <c r="C6" s="206"/>
+      <c r="D6" s="206"/>
+      <c r="E6" s="206"/>
+      <c r="F6" s="206"/>
+      <c r="G6" s="206"/>
+      <c r="H6" s="206"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="L6" s="3" t="s">
@@ -10224,10 +11164,10 @@
     </row>
     <row r="10" spans="1:26" ht="15">
       <c r="A10" s="1"/>
-      <c r="B10" s="192" t="s">
+      <c r="B10" s="205" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="193"/>
+      <c r="C10" s="206"/>
       <c r="D10" s="74" t="e">
         <f>(IS!M19/BS!M50)*(1-D11)</f>
         <v>#DIV/0!</v>
@@ -10264,10 +11204,10 @@
     </row>
     <row r="13" spans="1:26" ht="15">
       <c r="A13" s="1"/>
-      <c r="B13" s="192" t="s">
+      <c r="B13" s="205" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="193"/>
+      <c r="C13" s="206"/>
       <c r="D13" s="67">
         <f>INFO!C16/1000000</f>
         <v>0</v>
@@ -10298,10 +11238,10 @@
     </row>
     <row r="15" spans="1:26" ht="15">
       <c r="A15" s="1"/>
-      <c r="B15" s="192" t="s">
+      <c r="B15" s="205" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="193"/>
+      <c r="C15" s="206"/>
       <c r="D15" s="71">
         <f>D16+(D17*D18)</f>
         <v>0</v>
@@ -10318,10 +11258,10 @@
     </row>
     <row r="16" spans="1:26" ht="15">
       <c r="A16" s="1"/>
-      <c r="B16" s="192" t="s">
+      <c r="B16" s="205" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="193"/>
+      <c r="C16" s="206"/>
       <c r="D16" s="74">
         <f>INFO!C18 / 100</f>
         <v>0</v>
@@ -10368,10 +11308,10 @@
     </row>
     <row r="18" spans="1:14" ht="15">
       <c r="A18" s="1"/>
-      <c r="B18" s="192" t="s">
+      <c r="B18" s="205" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="193"/>
+      <c r="C18" s="206"/>
       <c r="D18" s="75">
         <f>D16*D17</f>
         <v>0</v>
@@ -10393,10 +11333,10 @@
     </row>
     <row r="20" spans="1:14" ht="15">
       <c r="A20" s="1"/>
-      <c r="B20" s="192" t="s">
+      <c r="B20" s="205" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="193"/>
+      <c r="C20" s="206"/>
       <c r="D20" s="67">
         <f>D13+D8</f>
         <v>0</v>
@@ -10493,13 +11433,13 @@
   <sheetData>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="8"/>
-      <c r="B2" s="198" t="e">
+      <c r="B2" s="211" t="e">
         <f>CONCATENATE(#REF!," Revenue Breakdown")</f>
         <v>#REF!</v>
       </c>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
+      <c r="C2" s="212"/>
+      <c r="D2" s="212"/>
+      <c r="E2" s="212"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -10521,10 +11461,10 @@
       <c r="X2" s="8"/>
     </row>
     <row r="4" spans="1:24" ht="15">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="209" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="193"/>
+      <c r="C4" s="206"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="19" t="e">
@@ -11662,10 +12602,10 @@
       </c>
     </row>
     <row r="57" spans="2:21" ht="15">
-      <c r="B57" s="196" t="s">
+      <c r="B57" s="209" t="s">
         <v>107</v>
       </c>
-      <c r="C57" s="193"/>
+      <c r="C57" s="206"/>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="19" t="e">
@@ -12352,12 +13292,12 @@
     </row>
     <row r="2" spans="1:25" ht="24">
       <c r="A2" s="97"/>
-      <c r="B2" s="206" t="s">
+      <c r="B2" s="219" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="207"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="207"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
       <c r="F2" s="98"/>
       <c r="G2" s="98"/>
       <c r="H2" s="98"/>
@@ -12394,10 +13334,10 @@
     </row>
     <row r="4" spans="1:25" ht="15">
       <c r="A4" s="1"/>
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="209" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="200"/>
+      <c r="C4" s="213"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -12429,8 +13369,8 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="197"/>
-      <c r="G5" s="193"/>
+      <c r="F5" s="210"/>
+      <c r="G5" s="206"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -12450,26 +13390,26 @@
     </row>
     <row r="6" spans="1:25" ht="15">
       <c r="A6" s="1"/>
-      <c r="B6" s="192" t="s">
+      <c r="B6" s="205" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="193"/>
-      <c r="D6" s="208"/>
-      <c r="E6" s="209"/>
-      <c r="F6" s="209"/>
-      <c r="G6" s="209"/>
-      <c r="H6" s="209"/>
-      <c r="I6" s="210"/>
+      <c r="C6" s="206"/>
+      <c r="D6" s="221"/>
+      <c r="E6" s="222"/>
+      <c r="F6" s="222"/>
+      <c r="G6" s="222"/>
+      <c r="H6" s="222"/>
+      <c r="I6" s="223"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="192" t="e">
+      <c r="K6" s="205" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L6" s="193"/>
-      <c r="M6" s="193"/>
-      <c r="N6" s="193"/>
-      <c r="O6" s="193"/>
-      <c r="P6" s="193"/>
+      <c r="L6" s="206"/>
+      <c r="M6" s="206"/>
+      <c r="N6" s="206"/>
+      <c r="O6" s="206"/>
+      <c r="P6" s="206"/>
       <c r="Q6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -12502,26 +13442,26 @@
       <c r="A8" s="97"/>
       <c r="B8" s="177"/>
       <c r="C8" s="177"/>
-      <c r="D8" s="201" t="s">
+      <c r="D8" s="214" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="202"/>
-      <c r="F8" s="202"/>
-      <c r="G8" s="202"/>
-      <c r="H8" s="202"/>
-      <c r="I8" s="202"/>
+      <c r="E8" s="215"/>
+      <c r="F8" s="215"/>
+      <c r="G8" s="215"/>
+      <c r="H8" s="215"/>
+      <c r="I8" s="215"/>
       <c r="J8" s="177"/>
-      <c r="K8" s="201" t="s">
+      <c r="K8" s="214" t="s">
         <v>125</v>
       </c>
-      <c r="L8" s="202"/>
-      <c r="M8" s="202"/>
+      <c r="L8" s="215"/>
+      <c r="M8" s="215"/>
       <c r="N8" s="177"/>
-      <c r="O8" s="201" t="s">
+      <c r="O8" s="214" t="s">
         <v>126</v>
       </c>
-      <c r="P8" s="202"/>
-      <c r="Q8" s="202"/>
+      <c r="P8" s="215"/>
+      <c r="Q8" s="215"/>
       <c r="R8" s="97"/>
     </row>
     <row r="9" spans="1:25" ht="16">
@@ -14097,11 +15037,11 @@
     </row>
     <row r="41" spans="1:18" ht="16">
       <c r="A41" s="97"/>
-      <c r="B41" s="211" t="str">
+      <c r="B41" s="224" t="str">
         <f>(B11&amp;" Valuation")</f>
         <v>0 Valuation</v>
       </c>
-      <c r="C41" s="200"/>
+      <c r="C41" s="213"/>
       <c r="D41" s="179"/>
       <c r="E41" s="179"/>
       <c r="F41" s="179"/>
@@ -14126,10 +15066,10 @@
     </row>
     <row r="42" spans="1:18" ht="16">
       <c r="A42" s="97"/>
-      <c r="B42" s="203" t="s">
+      <c r="B42" s="216" t="s">
         <v>143</v>
       </c>
-      <c r="C42" s="193"/>
+      <c r="C42" s="206"/>
       <c r="D42" s="97"/>
       <c r="E42" s="97"/>
       <c r="F42" s="97"/>
@@ -14188,10 +15128,10 @@
     </row>
     <row r="44" spans="1:18" ht="16">
       <c r="A44" s="97"/>
-      <c r="B44" s="203" t="s">
+      <c r="B44" s="216" t="s">
         <v>145</v>
       </c>
-      <c r="C44" s="193"/>
+      <c r="C44" s="206"/>
       <c r="D44" s="97"/>
       <c r="E44" s="97"/>
       <c r="F44" s="97"/>
@@ -14219,10 +15159,10 @@
     </row>
     <row r="45" spans="1:18" ht="16">
       <c r="A45" s="97"/>
-      <c r="B45" s="203" t="s">
+      <c r="B45" s="216" t="s">
         <v>146</v>
       </c>
-      <c r="C45" s="193"/>
+      <c r="C45" s="206"/>
       <c r="D45" s="97"/>
       <c r="E45" s="97"/>
       <c r="F45" s="97"/>
@@ -14250,10 +15190,10 @@
     </row>
     <row r="46" spans="1:18" ht="16">
       <c r="A46" s="97"/>
-      <c r="B46" s="204" t="s">
+      <c r="B46" s="217" t="s">
         <v>147</v>
       </c>
-      <c r="C46" s="205"/>
+      <c r="C46" s="218"/>
       <c r="D46" s="126"/>
       <c r="E46" s="126"/>
       <c r="F46" s="126"/>
@@ -14479,12 +15419,12 @@
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="2:23" ht="15.75" customHeight="1">
-      <c r="B2" s="198" t="e">
+      <c r="B2" s="211" t="e">
         <f>CONCATENATE(#REF!," EBITDA Multiple")</f>
         <v>#REF!</v>
       </c>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
+      <c r="C2" s="212"/>
+      <c r="D2" s="212"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -14538,10 +15478,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="192" t="s">
+      <c r="E4" s="205" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="193"/>
+      <c r="F4" s="206"/>
       <c r="G4" s="11">
         <f>Z84</f>
         <v>0</v>
@@ -14573,22 +15513,22 @@
       </c>
       <c r="C5" s="13">
         <f ca="1">TODAY()</f>
-        <v>45319</v>
+        <v>45330</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="192" t="s">
+      <c r="E5" s="205" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="193"/>
+      <c r="F5" s="206"/>
       <c r="G5" s="14" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="192" t="s">
+      <c r="I5" s="205" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="193"/>
+      <c r="J5" s="206"/>
       <c r="K5" s="15" t="e">
         <f>U84/G5-1</f>
         <v>#REF!</v>
@@ -14634,10 +15574,10 @@
       <c r="W6" s="1"/>
     </row>
     <row r="7" spans="2:23" ht="15">
-      <c r="B7" s="196" t="s">
+      <c r="B7" s="209" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="193"/>
+      <c r="C7" s="206"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -14666,10 +15606,10 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="197" t="s">
+      <c r="F8" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="193"/>
+      <c r="G8" s="206"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="10" t="s">
@@ -14678,10 +15618,10 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="197" t="s">
+      <c r="N8" s="210" t="s">
         <v>43</v>
       </c>
-      <c r="O8" s="193"/>
+      <c r="O8" s="206"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -14692,19 +15632,19 @@
       <c r="W8" s="1"/>
     </row>
     <row r="9" spans="2:23" ht="15">
-      <c r="B9" s="192" t="s">
+      <c r="B9" s="205" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="193"/>
+      <c r="C9" s="206"/>
       <c r="D9" s="2">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="192" t="e">
+      <c r="F9" s="205" t="e">
         <f>CONCATENATE("Revenue ", Q39)</f>
         <v>#REF!</v>
       </c>
-      <c r="G9" s="193"/>
+      <c r="G9" s="206"/>
       <c r="H9" s="2">
         <f>Q43-1%</f>
         <v>-0.01</v>
@@ -14714,11 +15654,11 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="192" t="e">
+      <c r="N9" s="205" t="e">
         <f>CONCATENATE("Revenue ", Q39)</f>
         <v>#REF!</v>
       </c>
-      <c r="O9" s="193"/>
+      <c r="O9" s="206"/>
       <c r="P9" s="2">
         <f>Q43+1%</f>
         <v>0.01</v>
@@ -14731,37 +15671,37 @@
       <c r="W9" s="1"/>
     </row>
     <row r="10" spans="2:23" ht="15">
-      <c r="B10" s="192" t="s">
+      <c r="B10" s="205" t="s">
         <v>151</v>
       </c>
-      <c r="C10" s="193"/>
+      <c r="C10" s="206"/>
       <c r="D10" s="16">
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="192" t="e">
+      <c r="F10" s="205" t="e">
         <f>CONCATENATE("Revenue ", Z39)</f>
         <v>#REF!</v>
       </c>
-      <c r="G10" s="193"/>
+      <c r="G10" s="206"/>
       <c r="H10" s="17">
         <v>0.03</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="192" t="e">
+      <c r="J10" s="205" t="e">
         <f>CONCATENATE("Revenue ", Z39)</f>
         <v>#REF!</v>
       </c>
-      <c r="K10" s="193"/>
+      <c r="K10" s="206"/>
       <c r="L10" s="18">
         <v>0.05</v>
       </c>
       <c r="M10" s="1"/>
-      <c r="N10" s="192" t="e">
+      <c r="N10" s="205" t="e">
         <f>CONCATENATE("Revenue ", Z39)</f>
         <v>#REF!</v>
       </c>
-      <c r="O10" s="193"/>
+      <c r="O10" s="206"/>
       <c r="P10" s="17">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -14904,20 +15844,20 @@
         <v>0.09</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="192" t="e">
+      <c r="J14" s="205" t="e">
         <f>CONCATENATE("CapEx ", Z39)</f>
         <v>#REF!</v>
       </c>
-      <c r="K14" s="193"/>
+      <c r="K14" s="206"/>
       <c r="L14" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="M14" s="1"/>
-      <c r="N14" s="192" t="e">
+      <c r="N14" s="205" t="e">
         <f>CONCATENATE("CapEx ", Z39)</f>
         <v>#REF!</v>
       </c>
-      <c r="O14" s="193"/>
+      <c r="O14" s="206"/>
       <c r="P14" s="17">
         <v>0.05</v>
       </c>
@@ -15004,10 +15944,10 @@
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="15">
-      <c r="B17" s="197" t="s">
+      <c r="B17" s="210" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="193"/>
+      <c r="C17" s="206"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -15115,10 +16055,10 @@
       <c r="A21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="196" t="s">
+      <c r="B21" s="209" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="193"/>
+      <c r="C21" s="206"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="19" t="e">
@@ -15410,10 +16350,10 @@
       <c r="W25" s="22"/>
     </row>
     <row r="26" spans="1:26" ht="15">
-      <c r="B26" s="195" t="s">
+      <c r="B26" s="208" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="193"/>
+      <c r="C26" s="206"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="24" t="e">
@@ -15753,10 +16693,10 @@
     </row>
     <row r="31" spans="1:26" ht="15">
       <c r="A31" s="1"/>
-      <c r="B31" s="192" t="s">
+      <c r="B31" s="205" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="193"/>
+      <c r="C31" s="206"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -15810,11 +16750,11 @@
     </row>
     <row r="32" spans="1:26" ht="15">
       <c r="A32" s="1"/>
-      <c r="B32" s="192" t="s">
+      <c r="B32" s="205" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="193"/>
-      <c r="D32" s="193"/>
+      <c r="C32" s="206"/>
+      <c r="D32" s="206"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -15867,10 +16807,10 @@
     </row>
     <row r="33" spans="1:26" ht="15">
       <c r="A33" s="1"/>
-      <c r="B33" s="192" t="s">
+      <c r="B33" s="205" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="193"/>
+      <c r="C33" s="206"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -16135,10 +17075,10 @@
     </row>
     <row r="37" spans="1:26" ht="15">
       <c r="A37" s="1"/>
-      <c r="B37" s="192" t="s">
+      <c r="B37" s="205" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="193"/>
+      <c r="C37" s="206"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -16192,11 +17132,11 @@
     </row>
     <row r="38" spans="1:26" ht="15">
       <c r="A38" s="1"/>
-      <c r="B38" s="192" t="s">
+      <c r="B38" s="205" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="193"/>
-      <c r="D38" s="193"/>
+      <c r="C38" s="206"/>
+      <c r="D38" s="206"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -16249,10 +17189,10 @@
     </row>
     <row r="39" spans="1:26" ht="15">
       <c r="A39" s="1"/>
-      <c r="B39" s="192" t="s">
+      <c r="B39" s="205" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="193"/>
+      <c r="C39" s="206"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -16397,7 +17337,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="15">
-      <c r="B2" s="212" t="s">
+      <c r="B2" s="225" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="149"/>
@@ -16413,7 +17353,7 @@
       <c r="M2" s="150"/>
     </row>
     <row r="3" spans="2:13" ht="14">
-      <c r="B3" s="213"/>
+      <c r="B3" s="226"/>
       <c r="C3" s="151"/>
       <c r="D3" s="152"/>
       <c r="E3" s="152"/>
@@ -17168,7 +18108,7 @@
   <dimension ref="A2:M52"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection sqref="A1:M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -17179,7 +18119,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="14">
-      <c r="B2" s="214" t="s">
+      <c r="B2" s="227" t="s">
         <v>182</v>
       </c>
       <c r="C2" s="163"/>
@@ -17195,7 +18135,7 @@
       <c r="M2" s="164"/>
     </row>
     <row r="3" spans="2:13">
-      <c r="B3" s="215"/>
+      <c r="B3" s="228"/>
       <c r="C3" s="165"/>
       <c r="D3" s="166"/>
       <c r="E3" s="166"/>
@@ -17993,7 +18933,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="15">
-      <c r="B2" s="212" t="s">
+      <c r="B2" s="225" t="s">
         <v>215</v>
       </c>
       <c r="C2" s="149"/>
@@ -18009,7 +18949,7 @@
       <c r="M2" s="150"/>
     </row>
     <row r="3" spans="2:13" ht="14">
-      <c r="B3" s="213"/>
+      <c r="B3" s="226"/>
       <c r="C3" s="151"/>
       <c r="D3" s="152"/>
       <c r="E3" s="152"/>

</xml_diff>

<commit_message>
Fix revenue estimate formulas.
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/FINDich.xlsx
+++ b/src/main/resources/templates/FINDich.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koko/IdeaProjects/FinanceProjects/stock-financial-report-analyzer/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D54E391-3DDC-954F-A88C-B04D4447ED55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73A4985-9C21-FA40-90D9-2DBA4F74F6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76680" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
@@ -2905,15 +2905,15 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2941,25 +2941,22 @@
     <xf numFmtId="0" fontId="39" fillId="9" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="171" fontId="32" fillId="0" borderId="45" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="171" fontId="32" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="172" fontId="32" fillId="0" borderId="45" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="172" fontId="32" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="9" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2977,14 +2974,17 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="32" fillId="0" borderId="45" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="32" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3939,7 +3939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A88C279-C091-A94C-B283-276290F6C98F}">
   <dimension ref="A2:H49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
@@ -3955,34 +3955,34 @@
       <c r="B2" s="227" t="s">
         <v>440</v>
       </c>
-      <c r="C2" s="236"/>
-      <c r="D2" s="236"/>
-      <c r="E2" s="236"/>
-      <c r="F2" s="236"/>
-      <c r="G2" s="236"/>
-      <c r="H2" s="236"/>
+      <c r="C2" s="235"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="235"/>
+      <c r="F2" s="235"/>
+      <c r="G2" s="235"/>
+      <c r="H2" s="235"/>
     </row>
     <row r="3" spans="2:8" ht="13" customHeight="1">
-      <c r="B3" s="237"/>
-      <c r="C3" s="238"/>
-      <c r="D3" s="238"/>
-      <c r="E3" s="238"/>
-      <c r="F3" s="238"/>
-      <c r="G3" s="238"/>
-      <c r="H3" s="238"/>
+      <c r="B3" s="236"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="237"/>
     </row>
     <row r="4" spans="2:8" ht="16" customHeight="1">
       <c r="B4" s="191" t="s">
         <v>441</v>
       </c>
-      <c r="C4" s="239" t="s">
+      <c r="C4" s="238" t="s">
         <v>468</v>
       </c>
-      <c r="D4" s="240"/>
-      <c r="E4" s="239" t="s">
+      <c r="D4" s="239"/>
+      <c r="E4" s="238" t="s">
         <v>469</v>
       </c>
-      <c r="F4" s="240"/>
+      <c r="F4" s="239"/>
       <c r="G4" s="196" t="s">
         <v>470</v>
       </c>
@@ -4003,10 +4003,10 @@
       <c r="B6" s="135" t="s">
         <v>446</v>
       </c>
-      <c r="C6" s="234"/>
-      <c r="D6" s="234"/>
-      <c r="E6" s="234"/>
-      <c r="F6" s="234"/>
+      <c r="C6" s="231"/>
+      <c r="D6" s="231"/>
+      <c r="E6" s="231"/>
+      <c r="F6" s="231"/>
       <c r="G6" s="148"/>
       <c r="H6" s="148"/>
     </row>
@@ -4014,10 +4014,10 @@
       <c r="B7" s="135" t="s">
         <v>445</v>
       </c>
-      <c r="C7" s="229"/>
-      <c r="D7" s="229"/>
-      <c r="E7" s="229"/>
-      <c r="F7" s="229"/>
+      <c r="C7" s="230"/>
+      <c r="D7" s="230"/>
+      <c r="E7" s="230"/>
+      <c r="F7" s="230"/>
       <c r="G7" s="147"/>
       <c r="H7" s="147"/>
     </row>
@@ -4025,10 +4025,10 @@
       <c r="B8" s="135" t="s">
         <v>444</v>
       </c>
-      <c r="C8" s="229"/>
-      <c r="D8" s="229"/>
-      <c r="E8" s="229"/>
-      <c r="F8" s="229"/>
+      <c r="C8" s="230"/>
+      <c r="D8" s="230"/>
+      <c r="E8" s="230"/>
+      <c r="F8" s="230"/>
       <c r="G8" s="147"/>
       <c r="H8" s="147"/>
     </row>
@@ -4036,10 +4036,10 @@
       <c r="B9" s="135" t="s">
         <v>443</v>
       </c>
-      <c r="C9" s="229"/>
-      <c r="D9" s="229"/>
-      <c r="E9" s="229"/>
-      <c r="F9" s="229"/>
+      <c r="C9" s="230"/>
+      <c r="D9" s="230"/>
+      <c r="E9" s="230"/>
+      <c r="F9" s="230"/>
       <c r="G9" s="147"/>
       <c r="H9" s="147"/>
     </row>
@@ -4047,10 +4047,10 @@
       <c r="B10" s="135" t="s">
         <v>442</v>
       </c>
-      <c r="C10" s="229"/>
-      <c r="D10" s="229"/>
-      <c r="E10" s="229"/>
-      <c r="F10" s="229"/>
+      <c r="C10" s="230"/>
+      <c r="D10" s="230"/>
+      <c r="E10" s="230"/>
+      <c r="F10" s="230"/>
       <c r="G10" s="147"/>
       <c r="H10" s="147"/>
     </row>
@@ -4067,14 +4067,14 @@
       <c r="B12" s="193" t="s">
         <v>447</v>
       </c>
-      <c r="C12" s="232" t="s">
+      <c r="C12" s="240" t="s">
         <v>468</v>
       </c>
-      <c r="D12" s="233"/>
-      <c r="E12" s="232" t="s">
+      <c r="D12" s="241"/>
+      <c r="E12" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="F12" s="233"/>
+      <c r="F12" s="241"/>
       <c r="G12" s="195" t="s">
         <v>470</v>
       </c>
@@ -4095,10 +4095,10 @@
       <c r="B14" s="135" t="s">
         <v>446</v>
       </c>
-      <c r="C14" s="234"/>
-      <c r="D14" s="234"/>
-      <c r="E14" s="234"/>
-      <c r="F14" s="234"/>
+      <c r="C14" s="231"/>
+      <c r="D14" s="231"/>
+      <c r="E14" s="231"/>
+      <c r="F14" s="231"/>
       <c r="G14" s="148"/>
       <c r="H14" s="148"/>
     </row>
@@ -4106,10 +4106,10 @@
       <c r="B15" s="135" t="s">
         <v>445</v>
       </c>
-      <c r="C15" s="235"/>
-      <c r="D15" s="235"/>
-      <c r="E15" s="235"/>
-      <c r="F15" s="235"/>
+      <c r="C15" s="242"/>
+      <c r="D15" s="242"/>
+      <c r="E15" s="242"/>
+      <c r="F15" s="242"/>
       <c r="G15" s="148"/>
       <c r="H15" s="148"/>
     </row>
@@ -4117,10 +4117,10 @@
       <c r="B16" s="135" t="s">
         <v>444</v>
       </c>
-      <c r="C16" s="235"/>
-      <c r="D16" s="235"/>
-      <c r="E16" s="235"/>
-      <c r="F16" s="235"/>
+      <c r="C16" s="242"/>
+      <c r="D16" s="242"/>
+      <c r="E16" s="242"/>
+      <c r="F16" s="242"/>
       <c r="G16" s="148"/>
       <c r="H16" s="148"/>
     </row>
@@ -4128,10 +4128,10 @@
       <c r="B17" s="135" t="s">
         <v>443</v>
       </c>
-      <c r="C17" s="235"/>
-      <c r="D17" s="235"/>
-      <c r="E17" s="235"/>
-      <c r="F17" s="235"/>
+      <c r="C17" s="242"/>
+      <c r="D17" s="242"/>
+      <c r="E17" s="242"/>
+      <c r="F17" s="242"/>
       <c r="G17" s="148"/>
       <c r="H17" s="148"/>
     </row>
@@ -4139,10 +4139,10 @@
       <c r="B18" s="135" t="s">
         <v>448</v>
       </c>
-      <c r="C18" s="235"/>
-      <c r="D18" s="235"/>
-      <c r="E18" s="235"/>
-      <c r="F18" s="235"/>
+      <c r="C18" s="242"/>
+      <c r="D18" s="242"/>
+      <c r="E18" s="242"/>
+      <c r="F18" s="242"/>
       <c r="G18" s="148"/>
       <c r="H18" s="148"/>
     </row>
@@ -4150,10 +4150,10 @@
       <c r="B19" s="135" t="s">
         <v>449</v>
       </c>
-      <c r="C19" s="235"/>
-      <c r="D19" s="235"/>
-      <c r="E19" s="235"/>
-      <c r="F19" s="235"/>
+      <c r="C19" s="242"/>
+      <c r="D19" s="242"/>
+      <c r="E19" s="242"/>
+      <c r="F19" s="242"/>
       <c r="G19" s="148"/>
       <c r="H19" s="148"/>
     </row>
@@ -4169,10 +4169,10 @@
       <c r="B21" s="137" t="s">
         <v>450</v>
       </c>
-      <c r="C21" s="232"/>
-      <c r="D21" s="233"/>
-      <c r="E21" s="232"/>
-      <c r="F21" s="233"/>
+      <c r="C21" s="240"/>
+      <c r="D21" s="241"/>
+      <c r="E21" s="240"/>
+      <c r="F21" s="241"/>
       <c r="G21" s="195"/>
       <c r="H21" s="195"/>
     </row>
@@ -4180,10 +4180,10 @@
       <c r="B22" s="135" t="s">
         <v>451</v>
       </c>
-      <c r="C22" s="241"/>
-      <c r="D22" s="241"/>
-      <c r="E22" s="241"/>
-      <c r="F22" s="241"/>
+      <c r="C22" s="229"/>
+      <c r="D22" s="229"/>
+      <c r="E22" s="229"/>
+      <c r="F22" s="229"/>
       <c r="G22" s="147"/>
       <c r="H22" s="147"/>
     </row>
@@ -4191,10 +4191,10 @@
       <c r="B23" s="135" t="s">
         <v>452</v>
       </c>
-      <c r="C23" s="229"/>
-      <c r="D23" s="229"/>
-      <c r="E23" s="229"/>
-      <c r="F23" s="229"/>
+      <c r="C23" s="230"/>
+      <c r="D23" s="230"/>
+      <c r="E23" s="230"/>
+      <c r="F23" s="230"/>
       <c r="G23" s="147"/>
       <c r="H23" s="147"/>
     </row>
@@ -4202,10 +4202,10 @@
       <c r="B24" s="135" t="s">
         <v>453</v>
       </c>
-      <c r="C24" s="229"/>
-      <c r="D24" s="229"/>
-      <c r="E24" s="229"/>
-      <c r="F24" s="229"/>
+      <c r="C24" s="230"/>
+      <c r="D24" s="230"/>
+      <c r="E24" s="230"/>
+      <c r="F24" s="230"/>
       <c r="G24" s="147"/>
       <c r="H24" s="147"/>
     </row>
@@ -4213,10 +4213,10 @@
       <c r="B25" s="135" t="s">
         <v>454</v>
       </c>
-      <c r="C25" s="229"/>
-      <c r="D25" s="229"/>
-      <c r="E25" s="229"/>
-      <c r="F25" s="229"/>
+      <c r="C25" s="230"/>
+      <c r="D25" s="230"/>
+      <c r="E25" s="230"/>
+      <c r="F25" s="230"/>
       <c r="G25" s="147"/>
       <c r="H25" s="147"/>
     </row>
@@ -4224,10 +4224,10 @@
       <c r="B26" s="135" t="s">
         <v>455</v>
       </c>
-      <c r="C26" s="229"/>
-      <c r="D26" s="229"/>
-      <c r="E26" s="229"/>
-      <c r="F26" s="229"/>
+      <c r="C26" s="230"/>
+      <c r="D26" s="230"/>
+      <c r="E26" s="230"/>
+      <c r="F26" s="230"/>
       <c r="G26" s="199"/>
       <c r="H26" s="199"/>
     </row>
@@ -4235,10 +4235,10 @@
       <c r="B27" s="135" t="s">
         <v>456</v>
       </c>
-      <c r="C27" s="229"/>
-      <c r="D27" s="229"/>
-      <c r="E27" s="229"/>
-      <c r="F27" s="229"/>
+      <c r="C27" s="230"/>
+      <c r="D27" s="230"/>
+      <c r="E27" s="230"/>
+      <c r="F27" s="230"/>
       <c r="G27" s="199"/>
       <c r="H27" s="199"/>
     </row>
@@ -4256,14 +4256,14 @@
       <c r="B29" s="189" t="s">
         <v>467</v>
       </c>
-      <c r="C29" s="232" t="s">
+      <c r="C29" s="240" t="s">
         <v>468</v>
       </c>
-      <c r="D29" s="233"/>
-      <c r="E29" s="232" t="s">
+      <c r="D29" s="241"/>
+      <c r="E29" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="F29" s="233"/>
+      <c r="F29" s="241"/>
       <c r="G29" s="195" t="s">
         <v>470</v>
       </c>
@@ -4286,10 +4286,10 @@
       <c r="B31" s="153" t="s">
         <v>472</v>
       </c>
-      <c r="C31" s="230"/>
-      <c r="D31" s="230"/>
-      <c r="E31" s="230"/>
-      <c r="F31" s="230"/>
+      <c r="C31" s="234"/>
+      <c r="D31" s="234"/>
+      <c r="E31" s="234"/>
+      <c r="F31" s="234"/>
       <c r="G31" s="197"/>
       <c r="H31" s="197"/>
     </row>
@@ -4298,10 +4298,10 @@
       <c r="B32" s="153" t="s">
         <v>473</v>
       </c>
-      <c r="C32" s="229"/>
-      <c r="D32" s="229"/>
-      <c r="E32" s="229"/>
-      <c r="F32" s="229"/>
+      <c r="C32" s="230"/>
+      <c r="D32" s="230"/>
+      <c r="E32" s="230"/>
+      <c r="F32" s="230"/>
       <c r="G32" s="197"/>
       <c r="H32" s="197"/>
     </row>
@@ -4310,10 +4310,10 @@
       <c r="B33" s="153" t="s">
         <v>474</v>
       </c>
-      <c r="C33" s="229"/>
-      <c r="D33" s="229"/>
-      <c r="E33" s="229"/>
-      <c r="F33" s="229"/>
+      <c r="C33" s="230"/>
+      <c r="D33" s="230"/>
+      <c r="E33" s="230"/>
+      <c r="F33" s="230"/>
       <c r="G33" s="197"/>
       <c r="H33" s="197"/>
     </row>
@@ -4322,10 +4322,10 @@
       <c r="B34" s="153" t="s">
         <v>475</v>
       </c>
-      <c r="C34" s="229"/>
-      <c r="D34" s="229"/>
-      <c r="E34" s="229"/>
-      <c r="F34" s="229"/>
+      <c r="C34" s="230"/>
+      <c r="D34" s="230"/>
+      <c r="E34" s="230"/>
+      <c r="F34" s="230"/>
       <c r="G34" s="197"/>
       <c r="H34" s="197"/>
     </row>
@@ -4334,10 +4334,10 @@
       <c r="B35" s="153" t="s">
         <v>476</v>
       </c>
-      <c r="C35" s="229"/>
-      <c r="D35" s="229"/>
-      <c r="E35" s="229"/>
-      <c r="F35" s="229"/>
+      <c r="C35" s="230"/>
+      <c r="D35" s="230"/>
+      <c r="E35" s="230"/>
+      <c r="F35" s="230"/>
       <c r="G35" s="197"/>
       <c r="H35" s="197"/>
     </row>
@@ -4355,10 +4355,10 @@
       <c r="B37" s="185" t="s">
         <v>457</v>
       </c>
-      <c r="C37" s="242"/>
-      <c r="D37" s="243"/>
-      <c r="E37" s="242"/>
-      <c r="F37" s="243"/>
+      <c r="C37" s="232"/>
+      <c r="D37" s="233"/>
+      <c r="E37" s="232"/>
+      <c r="F37" s="233"/>
       <c r="G37" s="198"/>
       <c r="H37" s="198"/>
     </row>
@@ -4366,10 +4366,10 @@
       <c r="B38" s="135" t="s">
         <v>458</v>
       </c>
-      <c r="C38" s="241"/>
-      <c r="D38" s="241"/>
-      <c r="E38" s="241"/>
-      <c r="F38" s="241"/>
+      <c r="C38" s="229"/>
+      <c r="D38" s="229"/>
+      <c r="E38" s="229"/>
+      <c r="F38" s="229"/>
       <c r="G38" s="147"/>
       <c r="H38" s="147"/>
     </row>
@@ -4377,10 +4377,10 @@
       <c r="B39" s="135" t="s">
         <v>459</v>
       </c>
-      <c r="C39" s="229"/>
-      <c r="D39" s="229"/>
-      <c r="E39" s="229"/>
-      <c r="F39" s="229"/>
+      <c r="C39" s="230"/>
+      <c r="D39" s="230"/>
+      <c r="E39" s="230"/>
+      <c r="F39" s="230"/>
       <c r="G39" s="147"/>
       <c r="H39" s="147"/>
     </row>
@@ -4388,10 +4388,10 @@
       <c r="B40" s="135" t="s">
         <v>460</v>
       </c>
-      <c r="C40" s="229"/>
-      <c r="D40" s="229"/>
-      <c r="E40" s="229"/>
-      <c r="F40" s="229"/>
+      <c r="C40" s="230"/>
+      <c r="D40" s="230"/>
+      <c r="E40" s="230"/>
+      <c r="F40" s="230"/>
       <c r="G40" s="147"/>
       <c r="H40" s="147"/>
     </row>
@@ -4399,10 +4399,10 @@
       <c r="B41" s="135" t="s">
         <v>461</v>
       </c>
-      <c r="C41" s="229"/>
-      <c r="D41" s="229"/>
-      <c r="E41" s="229"/>
-      <c r="F41" s="229"/>
+      <c r="C41" s="230"/>
+      <c r="D41" s="230"/>
+      <c r="E41" s="230"/>
+      <c r="F41" s="230"/>
       <c r="G41" s="147"/>
       <c r="H41" s="147"/>
     </row>
@@ -4420,14 +4420,14 @@
       <c r="B43" s="189" t="s">
         <v>462</v>
       </c>
-      <c r="C43" s="232" t="s">
+      <c r="C43" s="240" t="s">
         <v>468</v>
       </c>
-      <c r="D43" s="233"/>
-      <c r="E43" s="232" t="s">
+      <c r="D43" s="241"/>
+      <c r="E43" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="F43" s="233"/>
+      <c r="F43" s="241"/>
       <c r="G43" s="195" t="s">
         <v>470</v>
       </c>
@@ -4450,10 +4450,10 @@
       <c r="B45" s="153" t="s">
         <v>463</v>
       </c>
-      <c r="C45" s="230"/>
-      <c r="D45" s="230"/>
-      <c r="E45" s="230"/>
-      <c r="F45" s="230"/>
+      <c r="C45" s="234"/>
+      <c r="D45" s="234"/>
+      <c r="E45" s="234"/>
+      <c r="F45" s="234"/>
       <c r="G45" s="197"/>
       <c r="H45" s="197"/>
     </row>
@@ -4462,10 +4462,10 @@
       <c r="B46" s="153" t="s">
         <v>464</v>
       </c>
-      <c r="C46" s="231"/>
-      <c r="D46" s="231"/>
-      <c r="E46" s="231"/>
-      <c r="F46" s="231"/>
+      <c r="C46" s="243"/>
+      <c r="D46" s="243"/>
+      <c r="E46" s="243"/>
+      <c r="F46" s="243"/>
       <c r="G46" s="197"/>
       <c r="H46" s="197"/>
     </row>
@@ -4474,10 +4474,10 @@
       <c r="B47" s="153" t="s">
         <v>465</v>
       </c>
-      <c r="C47" s="231"/>
-      <c r="D47" s="231"/>
-      <c r="E47" s="231"/>
-      <c r="F47" s="231"/>
+      <c r="C47" s="243"/>
+      <c r="D47" s="243"/>
+      <c r="E47" s="243"/>
+      <c r="F47" s="243"/>
       <c r="G47" s="197"/>
       <c r="H47" s="197"/>
     </row>
@@ -4486,10 +4486,10 @@
       <c r="B48" s="153" t="s">
         <v>466</v>
       </c>
-      <c r="C48" s="231"/>
-      <c r="D48" s="231"/>
-      <c r="E48" s="231"/>
-      <c r="F48" s="231"/>
+      <c r="C48" s="243"/>
+      <c r="D48" s="243"/>
+      <c r="E48" s="243"/>
+      <c r="F48" s="243"/>
       <c r="G48" s="197"/>
       <c r="H48" s="197"/>
     </row>
@@ -4503,6 +4503,63 @@
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="C41:D41"/>
@@ -4519,63 +4576,6 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="B2:H3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6219,8 +6219,8 @@
   </sheetPr>
   <dimension ref="A1:AB89"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -6256,11 +6256,11 @@
     </row>
     <row r="2" spans="1:24" ht="21">
       <c r="A2" s="8"/>
-      <c r="B2" s="211" t="str">
+      <c r="B2" s="208" t="str">
         <f>CONCATENATE(INFO!C4, " ", "DCF")</f>
         <v xml:space="preserve"> DCF</v>
       </c>
-      <c r="C2" s="212"/>
+      <c r="C2" s="209"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -6321,7 +6321,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="205" t="s">
+      <c r="E4" s="207" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="206"/>
@@ -6361,7 +6361,7 @@
         <v>45330</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="205" t="s">
+      <c r="E5" s="207" t="s">
         <v>37</v>
       </c>
       <c r="F5" s="206"/>
@@ -6424,10 +6424,10 @@
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="209" t="s">
+      <c r="B7" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="213"/>
+      <c r="C7" s="211"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -6458,7 +6458,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="210" t="s">
+      <c r="F8" s="205" t="s">
         <v>41</v>
       </c>
       <c r="G8" s="206"/>
@@ -6470,7 +6470,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="210" t="s">
+      <c r="N8" s="205" t="s">
         <v>43</v>
       </c>
       <c r="O8" s="206"/>
@@ -6486,7 +6486,7 @@
     </row>
     <row r="9" spans="1:24" ht="15">
       <c r="A9" s="1"/>
-      <c r="B9" s="205" t="s">
+      <c r="B9" s="207" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="206"/>
@@ -6494,28 +6494,28 @@
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="205" t="e">
+      <c r="F9" s="207" t="e">
         <f>CONCATENATE("Revenue", " ",Q43)</f>
         <v>#VALUE!</v>
       </c>
       <c r="G9" s="206"/>
       <c r="H9" s="2" t="e">
         <f>Q47-1%</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="205" t="e">
+      <c r="N9" s="207" t="e">
         <f>CONCATENATE("Revenue ", Q43)</f>
         <v>#VALUE!</v>
       </c>
       <c r="O9" s="206"/>
       <c r="P9" s="2" t="e">
         <f>Q47+1%</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -6527,7 +6527,7 @@
     </row>
     <row r="10" spans="1:24" ht="15">
       <c r="A10" s="1"/>
-      <c r="B10" s="205" t="s">
+      <c r="B10" s="207" t="s">
         <v>45</v>
       </c>
       <c r="C10" s="206"/>
@@ -6535,7 +6535,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="205" t="e">
+      <c r="F10" s="207" t="e">
         <f>CONCATENATE("Revenue ", Z43)</f>
         <v>#VALUE!</v>
       </c>
@@ -6544,7 +6544,7 @@
         <v>0.03</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="205" t="e">
+      <c r="J10" s="207" t="e">
         <f>CONCATENATE("Revenue ", Z43)</f>
         <v>#VALUE!</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>0.05</v>
       </c>
       <c r="M10" s="1"/>
-      <c r="N10" s="205" t="e">
+      <c r="N10" s="207" t="e">
         <f>CONCATENATE("Revenue ", Z43)</f>
         <v>#VALUE!</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>0.09</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="205" t="e">
+      <c r="J14" s="207" t="e">
         <f>CONCATENATE("CapEx ", Z43)</f>
         <v>#VALUE!</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="M14" s="1"/>
-      <c r="N14" s="205" t="e">
+      <c r="N14" s="207" t="e">
         <f>CONCATENATE("CapEx ", Z43)</f>
         <v>#VALUE!</v>
       </c>
@@ -6814,7 +6814,7 @@
     </row>
     <row r="17" spans="1:24" ht="15">
       <c r="A17" s="1"/>
-      <c r="B17" s="210" t="s">
+      <c r="B17" s="205" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="206"/>
@@ -6932,7 +6932,7 @@
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="209" t="s">
+      <c r="B21" s="210" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="206"/>
@@ -7060,16 +7060,16 @@
         <v>0</v>
       </c>
       <c r="Q22" s="21" t="e">
-        <f>IF(ISBLANK(U22), IF(ISBLANK(#REF!), O22*(1+AVERAGE($G$23:O23)),#REF!/ 1000000), U22)</f>
-        <v>#REF!</v>
+        <f>IF(ISBLANK(U22),IF(OR(ISBLANK(RESEARCH!G15),RESEARCH!G13&lt;&gt;Q21),IF(OR(ISBLANK(RESEARCH!H15),RESEARCH!H13&lt;&gt;Q21),O22*(1+AVERAGE($G$23:O23)),RESEARCH!H15/1000000),RESEARCH!G15/1000000),U22)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="R22" s="20" t="e">
-        <f>IF(ISBLANK(V22), IF(ISBLANK(#REF!), Q22*(1+AVERAGE($G$23:O23, Q23)),#REF!/ 1000000), V22)</f>
-        <v>#REF!</v>
+        <f>IF(ISBLANK(V22), IF(OR(ISBLANK(RESEARCH!H15),RESEARCH!H13&lt;&gt;R21), Q22*(1+AVERAGE($G$23:O23,Q23)), RESEARCH!H15/1000000), V22)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="S22" s="20" t="e">
-        <f>IF(ISBLANK(W22), IF(ISBLANK(#REF!), R22*(1+AVERAGE($G$23:O23,Q23:R23)),#REF!/ 1000000), W22)</f>
-        <v>#REF!</v>
+        <f>IF(ISBLANK(W22), R22*(1+AVERAGE($G$23:O23,Q23:R23)), W22)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="T22" s="20"/>
       <c r="U22" s="22"/>
@@ -7124,15 +7124,15 @@
       <c r="P23" s="25"/>
       <c r="Q23" s="25" t="e">
         <f>(Q22/O22)-1</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R23" s="24" t="e">
         <f t="shared" ref="R23:S23" si="3">(R22/Q22)-1</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S23" s="24" t="e">
         <f t="shared" si="3"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T23" s="24"/>
       <c r="U23" s="26"/>
@@ -7232,7 +7232,7 @@
     </row>
     <row r="26" spans="1:24" ht="15">
       <c r="A26" s="1"/>
-      <c r="B26" s="208" t="s">
+      <c r="B26" s="212" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="206"/>
@@ -7465,7 +7465,7 @@
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="209" t="s">
+      <c r="B31" s="210" t="s">
         <v>60</v>
       </c>
       <c r="C31" s="206"/>
@@ -7612,7 +7612,7 @@
     </row>
     <row r="33" spans="1:26" ht="15">
       <c r="A33" s="1"/>
-      <c r="B33" s="208" t="s">
+      <c r="B33" s="212" t="s">
         <v>58</v>
       </c>
       <c r="C33" s="206"/>
@@ -7664,15 +7664,15 @@
       </c>
       <c r="Q33" s="25" t="e">
         <f t="shared" si="8"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R33" s="24" t="e">
         <f t="shared" si="8"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S33" s="24" t="e">
         <f t="shared" si="8"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T33" s="1"/>
       <c r="U33" s="28"/>
@@ -7682,7 +7682,7 @@
     </row>
     <row r="34" spans="1:26" ht="15">
       <c r="A34" s="1"/>
-      <c r="B34" s="208" t="s">
+      <c r="B34" s="212" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="206"/>
@@ -7764,7 +7764,7 @@
     </row>
     <row r="36" spans="1:26" ht="15">
       <c r="A36" s="1"/>
-      <c r="B36" s="205" t="s">
+      <c r="B36" s="207" t="s">
         <v>62</v>
       </c>
       <c r="C36" s="206"/>
@@ -7834,7 +7834,7 @@
     </row>
     <row r="37" spans="1:26" ht="15">
       <c r="A37" s="1"/>
-      <c r="B37" s="208" t="s">
+      <c r="B37" s="212" t="s">
         <v>58</v>
       </c>
       <c r="C37" s="206"/>
@@ -7886,15 +7886,15 @@
       </c>
       <c r="Q37" s="25" t="e">
         <f t="shared" si="10"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R37" s="24" t="e">
         <f t="shared" si="10"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S37" s="24" t="e">
         <f t="shared" si="10"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
@@ -7931,7 +7931,7 @@
     </row>
     <row r="39" spans="1:26" ht="15">
       <c r="A39" s="1"/>
-      <c r="B39" s="205" t="s">
+      <c r="B39" s="207" t="s">
         <v>63</v>
       </c>
       <c r="C39" s="206"/>
@@ -7994,7 +7994,7 @@
     </row>
     <row r="40" spans="1:26" ht="15">
       <c r="A40" s="1"/>
-      <c r="B40" s="208" t="s">
+      <c r="B40" s="212" t="s">
         <v>58</v>
       </c>
       <c r="C40" s="206"/>
@@ -8057,7 +8057,7 @@
     </row>
     <row r="41" spans="1:26" ht="15">
       <c r="A41" s="1"/>
-      <c r="B41" s="208" t="s">
+      <c r="B41" s="212" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="206"/>
@@ -8305,43 +8305,43 @@
       </c>
       <c r="Q44" s="38" t="e">
         <f ca="1">O44*(1+Q45)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R44" s="38" t="e">
         <f t="shared" ref="R44:Z44" ca="1" si="17">Q44*(1+R45)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S44" s="38" t="e">
         <f t="shared" ca="1" si="17"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T44" s="38" t="e">
         <f t="shared" ca="1" si="17"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U44" s="38" t="e">
         <f t="shared" ca="1" si="17"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V44" s="38" t="e">
         <f t="shared" ca="1" si="17"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="W44" s="38" t="e">
         <f t="shared" ca="1" si="17"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X44" s="38" t="e">
         <f t="shared" ca="1" si="17"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Y44" s="38" t="e">
         <f t="shared" ca="1" si="17"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z44" s="38" t="e">
         <f t="shared" ca="1" si="17"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="45" spans="1:26" ht="15">
@@ -8392,39 +8392,39 @@
       <c r="P45" s="40"/>
       <c r="Q45" s="25" t="e">
         <f t="shared" ref="Q45:Z45" ca="1" si="19">OFFSET(Q45,$D$9,0)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R45" s="25" t="e">
         <f t="shared" ca="1" si="19"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S45" s="25" t="e">
         <f t="shared" ca="1" si="19"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T45" s="41" t="e">
         <f t="shared" ca="1" si="19"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U45" s="41" t="e">
         <f t="shared" ca="1" si="19"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V45" s="41" t="e">
         <f t="shared" ca="1" si="19"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="W45" s="41" t="e">
         <f t="shared" ca="1" si="19"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X45" s="41" t="e">
         <f t="shared" ca="1" si="19"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Y45" s="41" t="e">
         <f t="shared" ca="1" si="19"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z45" s="40">
         <f t="shared" ca="1" si="19"/>
@@ -8433,7 +8433,7 @@
     </row>
     <row r="46" spans="1:26" ht="15">
       <c r="A46" s="1"/>
-      <c r="B46" s="205" t="s">
+      <c r="B46" s="207" t="s">
         <v>41</v>
       </c>
       <c r="C46" s="206"/>
@@ -8449,39 +8449,39 @@
       <c r="P46" s="27"/>
       <c r="Q46" s="42" t="e">
         <f>H9</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R46" s="43" t="e">
         <f t="shared" ref="R46:S46" si="20">Q46-(Q47-R47)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S46" s="43" t="e">
         <f t="shared" si="20"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T46" s="43" t="e">
         <f t="shared" ref="T46:Y46" si="21">S46-(($S$46-$Z$46)/($Z$43-$S$43))</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U46" s="43" t="e">
         <f t="shared" si="21"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V46" s="43" t="e">
         <f t="shared" si="21"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="W46" s="43" t="e">
         <f t="shared" si="21"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X46" s="43" t="e">
         <f t="shared" si="21"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Y46" s="43" t="e">
         <f t="shared" si="21"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z46" s="44">
         <f>H10</f>
@@ -8490,7 +8490,7 @@
     </row>
     <row r="47" spans="1:26" ht="15">
       <c r="A47" s="1"/>
-      <c r="B47" s="205" t="s">
+      <c r="B47" s="207" t="s">
         <v>65</v>
       </c>
       <c r="C47" s="206"/>
@@ -8506,39 +8506,39 @@
       <c r="P47" s="27"/>
       <c r="Q47" s="45" t="e">
         <f t="shared" ref="Q47:S47" si="22">Q23</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R47" s="45" t="e">
         <f t="shared" si="22"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S47" s="45" t="e">
         <f t="shared" si="22"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T47" s="43" t="e">
         <f t="shared" ref="T47:Y47" si="23">S47-(($S$47-$Z$47)/($Z$43-$S$43))</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U47" s="46" t="e">
         <f t="shared" si="23"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V47" s="46" t="e">
         <f t="shared" si="23"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="W47" s="46" t="e">
         <f t="shared" si="23"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X47" s="46" t="e">
         <f t="shared" si="23"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Y47" s="46" t="e">
         <f t="shared" si="23"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z47" s="47">
         <f>L10</f>
@@ -8547,7 +8547,7 @@
     </row>
     <row r="48" spans="1:26" ht="15">
       <c r="A48" s="1"/>
-      <c r="B48" s="205" t="s">
+      <c r="B48" s="207" t="s">
         <v>43</v>
       </c>
       <c r="C48" s="206"/>
@@ -8563,39 +8563,39 @@
       <c r="P48" s="27"/>
       <c r="Q48" s="42" t="e">
         <f>P9</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R48" s="43" t="e">
         <f t="shared" ref="R48:S48" si="24">Q48+(R47-Q47)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S48" s="43" t="e">
         <f t="shared" si="24"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T48" s="43" t="e">
         <f t="shared" ref="T48:Y48" si="25">S48-(($S$48-$Z$48)/($Z$43-$S$43))</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U48" s="46" t="e">
         <f t="shared" si="25"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V48" s="46" t="e">
         <f t="shared" si="25"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="W48" s="46" t="e">
         <f t="shared" si="25"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X48" s="46" t="e">
         <f t="shared" si="25"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Y48" s="46" t="e">
         <f t="shared" si="25"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z48" s="47">
         <f>P10</f>
@@ -8815,7 +8815,7 @@
     </row>
     <row r="52" spans="1:26" ht="15">
       <c r="A52" s="1"/>
-      <c r="B52" s="205" t="s">
+      <c r="B52" s="207" t="s">
         <v>41</v>
       </c>
       <c r="C52" s="206"/>
@@ -8872,7 +8872,7 @@
     </row>
     <row r="53" spans="1:26" ht="15">
       <c r="A53" s="1"/>
-      <c r="B53" s="205" t="s">
+      <c r="B53" s="207" t="s">
         <v>65</v>
       </c>
       <c r="C53" s="206"/>
@@ -8929,7 +8929,7 @@
     </row>
     <row r="54" spans="1:26" ht="15">
       <c r="A54" s="1"/>
-      <c r="B54" s="205" t="s">
+      <c r="B54" s="207" t="s">
         <v>43</v>
       </c>
       <c r="C54" s="206"/>
@@ -9197,7 +9197,7 @@
     </row>
     <row r="58" spans="1:26" ht="15">
       <c r="A58" s="1"/>
-      <c r="B58" s="205" t="s">
+      <c r="B58" s="207" t="s">
         <v>41</v>
       </c>
       <c r="C58" s="206"/>
@@ -9254,7 +9254,7 @@
     </row>
     <row r="59" spans="1:26" ht="15">
       <c r="A59" s="1"/>
-      <c r="B59" s="205" t="s">
+      <c r="B59" s="207" t="s">
         <v>65</v>
       </c>
       <c r="C59" s="206"/>
@@ -9311,7 +9311,7 @@
     </row>
     <row r="60" spans="1:26" ht="15">
       <c r="A60" s="1"/>
-      <c r="B60" s="205" t="s">
+      <c r="B60" s="207" t="s">
         <v>43</v>
       </c>
       <c r="C60" s="206"/>
@@ -9536,43 +9536,43 @@
       </c>
       <c r="Q64" s="63" t="e">
         <f t="shared" ref="Q64:Z64" ca="1" si="46">Q44*Q65</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R64" s="63" t="e">
         <f t="shared" ca="1" si="46"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S64" s="63" t="e">
         <f t="shared" ca="1" si="46"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T64" s="63" t="e">
         <f t="shared" ca="1" si="46"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U64" s="63" t="e">
         <f t="shared" ca="1" si="46"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V64" s="63" t="e">
         <f t="shared" ca="1" si="46"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="W64" s="63" t="e">
         <f t="shared" ca="1" si="46"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X64" s="63" t="e">
         <f t="shared" ca="1" si="46"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Y64" s="63" t="e">
         <f t="shared" ca="1" si="46"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z64" s="63" t="e">
         <f t="shared" ca="1" si="46"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="65" spans="1:28" ht="15">
@@ -9670,7 +9670,7 @@
     </row>
     <row r="66" spans="1:28" ht="15">
       <c r="A66" s="1"/>
-      <c r="B66" s="205" t="s">
+      <c r="B66" s="207" t="s">
         <v>41</v>
       </c>
       <c r="C66" s="206"/>
@@ -9730,7 +9730,7 @@
     </row>
     <row r="67" spans="1:28" ht="15">
       <c r="A67" s="1"/>
-      <c r="B67" s="205" t="s">
+      <c r="B67" s="207" t="s">
         <v>65</v>
       </c>
       <c r="C67" s="206"/>
@@ -9790,7 +9790,7 @@
     </row>
     <row r="68" spans="1:28" ht="15">
       <c r="A68" s="1"/>
-      <c r="B68" s="205" t="s">
+      <c r="B68" s="207" t="s">
         <v>43</v>
       </c>
       <c r="C68" s="206"/>
@@ -9930,43 +9930,43 @@
       </c>
       <c r="Q70" s="63" t="e">
         <f t="shared" ref="Q70:Z70" ca="1" si="53">Q44*Q71</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R70" s="63" t="e">
         <f t="shared" ca="1" si="53"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S70" s="63" t="e">
         <f t="shared" ca="1" si="53"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T70" s="63" t="e">
         <f t="shared" ca="1" si="53"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U70" s="63" t="e">
         <f t="shared" ca="1" si="53"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V70" s="63" t="e">
         <f t="shared" ca="1" si="53"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="W70" s="63" t="e">
         <f t="shared" ca="1" si="53"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X70" s="63" t="e">
         <f t="shared" ca="1" si="53"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Y70" s="63" t="e">
         <f t="shared" ca="1" si="53"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z70" s="63" t="e">
         <f t="shared" ca="1" si="53"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="71" spans="1:28" ht="15">
@@ -10023,39 +10023,39 @@
       </c>
       <c r="Q71" s="40" t="e">
         <f t="shared" ref="Q71:Z71" ca="1" si="55">OFFSET(Q71,$D$13,0)</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R71" s="40" t="e">
         <f t="shared" ca="1" si="55"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S71" s="40" t="e">
         <f t="shared" ca="1" si="55"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T71" s="41" t="e">
         <f t="shared" ca="1" si="55"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U71" s="41" t="e">
         <f t="shared" ca="1" si="55"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V71" s="41" t="e">
         <f t="shared" ca="1" si="55"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="W71" s="41" t="e">
         <f t="shared" ca="1" si="55"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X71" s="41" t="e">
         <f t="shared" ca="1" si="55"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Y71" s="41" t="e">
         <f t="shared" ca="1" si="55"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z71" s="40">
         <f t="shared" ca="1" si="55"/>
@@ -10067,7 +10067,7 @@
     </row>
     <row r="72" spans="1:28" ht="15">
       <c r="A72" s="1"/>
-      <c r="B72" s="205" t="s">
+      <c r="B72" s="207" t="s">
         <v>41</v>
       </c>
       <c r="C72" s="206"/>
@@ -10086,39 +10086,39 @@
       <c r="P72" s="29"/>
       <c r="Q72" s="55" t="e">
         <f>Q73</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R72" s="56" t="e">
         <f t="shared" ref="R72:S72" si="56">Q72+$AB$72</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S72" s="56" t="e">
         <f t="shared" si="56"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T72" s="49" t="e">
         <f t="shared" ref="T72:Y72" si="57">S72-(($S$72-$Z$72)/($Z$43-$S$43))</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U72" s="49" t="e">
         <f t="shared" si="57"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V72" s="49" t="e">
         <f t="shared" si="57"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="W72" s="49" t="e">
         <f t="shared" si="57"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X72" s="49" t="e">
         <f t="shared" si="57"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Y72" s="49" t="e">
         <f t="shared" si="57"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z72" s="44">
         <f>H14</f>
@@ -10131,7 +10131,7 @@
     </row>
     <row r="73" spans="1:28" ht="15">
       <c r="A73" s="1"/>
-      <c r="B73" s="205" t="s">
+      <c r="B73" s="207" t="s">
         <v>65</v>
       </c>
       <c r="C73" s="206"/>
@@ -10150,39 +10150,39 @@
       <c r="P73" s="29"/>
       <c r="Q73" s="59" t="e">
         <f>Q37</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R73" s="47" t="e">
         <f t="shared" ref="R73:S73" si="58">Q73</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S73" s="47" t="e">
         <f t="shared" si="58"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T73" s="46" t="e">
         <f t="shared" ref="T73:Y73" si="59">S73-(($S$73-$Z$73)/($Z$43-$S$43))</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U73" s="46" t="e">
         <f t="shared" si="59"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V73" s="46" t="e">
         <f t="shared" si="59"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="W73" s="46" t="e">
         <f t="shared" si="59"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X73" s="46" t="e">
         <f t="shared" si="59"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Y73" s="46" t="e">
         <f t="shared" si="59"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z73" s="47">
         <f>L14</f>
@@ -10191,7 +10191,7 @@
     </row>
     <row r="74" spans="1:28" ht="15">
       <c r="A74" s="1"/>
-      <c r="B74" s="205" t="s">
+      <c r="B74" s="207" t="s">
         <v>43</v>
       </c>
       <c r="C74" s="206"/>
@@ -10210,39 +10210,39 @@
       <c r="P74" s="29"/>
       <c r="Q74" s="59" t="e">
         <f>Q73</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R74" s="58" t="e">
         <f t="shared" ref="R74:S74" si="60">Q74+$AB$74</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S74" s="58" t="e">
         <f t="shared" si="60"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T74" s="46" t="e">
         <f t="shared" ref="T74:Y74" si="61">S74-(($S$74-$Z$74)/($Z$43-$S$43))</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U74" s="46" t="e">
         <f t="shared" si="61"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V74" s="46" t="e">
         <f t="shared" si="61"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="W74" s="46" t="e">
         <f t="shared" si="61"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X74" s="46" t="e">
         <f t="shared" si="61"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Y74" s="46" t="e">
         <f t="shared" si="61"/>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z74" s="58">
         <f>P14</f>
@@ -10282,7 +10282,7 @@
     </row>
     <row r="76" spans="1:28" ht="15">
       <c r="A76" s="1"/>
-      <c r="B76" s="205" t="s">
+      <c r="B76" s="207" t="s">
         <v>63</v>
       </c>
       <c r="C76" s="206"/>
@@ -10496,7 +10496,7 @@
     </row>
     <row r="79" spans="1:28" ht="15">
       <c r="A79" s="1"/>
-      <c r="B79" s="207" t="s">
+      <c r="B79" s="213" t="s">
         <v>70</v>
       </c>
       <c r="C79" s="206"/>
@@ -10556,7 +10556,7 @@
     </row>
     <row r="80" spans="1:28" ht="15">
       <c r="A80" s="1"/>
-      <c r="B80" s="205" t="s">
+      <c r="B80" s="207" t="s">
         <v>71</v>
       </c>
       <c r="C80" s="206"/>
@@ -10612,7 +10612,7 @@
     </row>
     <row r="81" spans="1:26" ht="15">
       <c r="A81" s="1"/>
-      <c r="B81" s="205" t="s">
+      <c r="B81" s="207" t="s">
         <v>72</v>
       </c>
       <c r="C81" s="206"/>
@@ -10644,7 +10644,7 @@
     </row>
     <row r="82" spans="1:26" ht="15">
       <c r="A82" s="1"/>
-      <c r="B82" s="205" t="s">
+      <c r="B82" s="207" t="s">
         <v>73</v>
       </c>
       <c r="C82" s="206"/>
@@ -10676,7 +10676,7 @@
     </row>
     <row r="83" spans="1:26" ht="15">
       <c r="A83" s="1"/>
-      <c r="B83" s="205" t="s">
+      <c r="B83" s="207" t="s">
         <v>74</v>
       </c>
       <c r="C83" s="206"/>
@@ -10772,7 +10772,7 @@
     </row>
     <row r="86" spans="1:26" ht="15">
       <c r="A86" s="1"/>
-      <c r="B86" s="205" t="s">
+      <c r="B86" s="207" t="s">
         <v>77</v>
       </c>
       <c r="C86" s="206"/>
@@ -10804,7 +10804,7 @@
     </row>
     <row r="87" spans="1:26" ht="15">
       <c r="A87" s="1"/>
-      <c r="B87" s="205" t="s">
+      <c r="B87" s="207" t="s">
         <v>78</v>
       </c>
       <c r="C87" s="206"/>
@@ -10836,7 +10836,7 @@
     </row>
     <row r="88" spans="1:26" ht="15">
       <c r="A88" s="1"/>
-      <c r="B88" s="205" t="s">
+      <c r="B88" s="207" t="s">
         <v>79</v>
       </c>
       <c r="C88" s="206"/>
@@ -10894,39 +10894,11 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
     <mergeCell ref="B59:D59"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B66:C66"/>
@@ -10939,11 +10911,39 @@
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B79:D79"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J14:K14"/>
   </mergeCells>
   <conditionalFormatting sqref="F76:P76">
     <cfRule type="cellIs" dxfId="13" priority="4" operator="greaterThanOrEqual">
@@ -11066,7 +11066,7 @@
     </row>
     <row r="5" spans="1:26" ht="15">
       <c r="A5" s="1"/>
-      <c r="B5" s="210" t="s">
+      <c r="B5" s="205" t="s">
         <v>80</v>
       </c>
       <c r="C5" s="206"/>
@@ -11080,7 +11080,7 @@
     </row>
     <row r="6" spans="1:26" ht="15">
       <c r="A6" s="1"/>
-      <c r="B6" s="210" t="s">
+      <c r="B6" s="205" t="s">
         <v>81</v>
       </c>
       <c r="C6" s="206"/>
@@ -11164,7 +11164,7 @@
     </row>
     <row r="10" spans="1:26" ht="15">
       <c r="A10" s="1"/>
-      <c r="B10" s="205" t="s">
+      <c r="B10" s="207" t="s">
         <v>87</v>
       </c>
       <c r="C10" s="206"/>
@@ -11204,7 +11204,7 @@
     </row>
     <row r="13" spans="1:26" ht="15">
       <c r="A13" s="1"/>
-      <c r="B13" s="205" t="s">
+      <c r="B13" s="207" t="s">
         <v>77</v>
       </c>
       <c r="C13" s="206"/>
@@ -11238,7 +11238,7 @@
     </row>
     <row r="15" spans="1:26" ht="15">
       <c r="A15" s="1"/>
-      <c r="B15" s="205" t="s">
+      <c r="B15" s="207" t="s">
         <v>90</v>
       </c>
       <c r="C15" s="206"/>
@@ -11258,7 +11258,7 @@
     </row>
     <row r="16" spans="1:26" ht="15">
       <c r="A16" s="1"/>
-      <c r="B16" s="205" t="s">
+      <c r="B16" s="207" t="s">
         <v>92</v>
       </c>
       <c r="C16" s="206"/>
@@ -11308,7 +11308,7 @@
     </row>
     <row r="18" spans="1:14" ht="15">
       <c r="A18" s="1"/>
-      <c r="B18" s="205" t="s">
+      <c r="B18" s="207" t="s">
         <v>83</v>
       </c>
       <c r="C18" s="206"/>
@@ -11333,7 +11333,7 @@
     </row>
     <row r="20" spans="1:14" ht="15">
       <c r="A20" s="1"/>
-      <c r="B20" s="205" t="s">
+      <c r="B20" s="207" t="s">
         <v>96</v>
       </c>
       <c r="C20" s="206"/>
@@ -11433,13 +11433,13 @@
   <sheetData>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="8"/>
-      <c r="B2" s="211" t="e">
+      <c r="B2" s="208" t="e">
         <f>CONCATENATE(#REF!," Revenue Breakdown")</f>
         <v>#REF!</v>
       </c>
-      <c r="C2" s="212"/>
-      <c r="D2" s="212"/>
-      <c r="E2" s="212"/>
+      <c r="C2" s="209"/>
+      <c r="D2" s="209"/>
+      <c r="E2" s="209"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -11461,7 +11461,7 @@
       <c r="X2" s="8"/>
     </row>
     <row r="4" spans="1:24" ht="15">
-      <c r="B4" s="209" t="s">
+      <c r="B4" s="210" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="206"/>
@@ -12602,7 +12602,7 @@
       </c>
     </row>
     <row r="57" spans="2:21" ht="15">
-      <c r="B57" s="209" t="s">
+      <c r="B57" s="210" t="s">
         <v>107</v>
       </c>
       <c r="C57" s="206"/>
@@ -13334,10 +13334,10 @@
     </row>
     <row r="4" spans="1:25" ht="15">
       <c r="A4" s="1"/>
-      <c r="B4" s="209" t="s">
+      <c r="B4" s="210" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="213"/>
+      <c r="C4" s="211"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -13369,7 +13369,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="210"/>
+      <c r="F5" s="205"/>
       <c r="G5" s="206"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -13390,7 +13390,7 @@
     </row>
     <row r="6" spans="1:25" ht="15">
       <c r="A6" s="1"/>
-      <c r="B6" s="205" t="s">
+      <c r="B6" s="207" t="s">
         <v>124</v>
       </c>
       <c r="C6" s="206"/>
@@ -13401,7 +13401,7 @@
       <c r="H6" s="222"/>
       <c r="I6" s="223"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="205" t="e">
+      <c r="K6" s="207" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -15041,7 +15041,7 @@
         <f>(B11&amp;" Valuation")</f>
         <v>0 Valuation</v>
       </c>
-      <c r="C41" s="213"/>
+      <c r="C41" s="211"/>
       <c r="D41" s="179"/>
       <c r="E41" s="179"/>
       <c r="F41" s="179"/>
@@ -15419,12 +15419,12 @@
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="2:23" ht="15.75" customHeight="1">
-      <c r="B2" s="211" t="e">
+      <c r="B2" s="208" t="e">
         <f>CONCATENATE(#REF!," EBITDA Multiple")</f>
         <v>#REF!</v>
       </c>
-      <c r="C2" s="212"/>
-      <c r="D2" s="212"/>
+      <c r="C2" s="209"/>
+      <c r="D2" s="209"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -15478,7 +15478,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="205" t="s">
+      <c r="E4" s="207" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="206"/>
@@ -15516,7 +15516,7 @@
         <v>45330</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="205" t="s">
+      <c r="E5" s="207" t="s">
         <v>37</v>
       </c>
       <c r="F5" s="206"/>
@@ -15525,7 +15525,7 @@
         <v>#REF!</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="205" t="s">
+      <c r="I5" s="207" t="s">
         <v>38</v>
       </c>
       <c r="J5" s="206"/>
@@ -15574,7 +15574,7 @@
       <c r="W6" s="1"/>
     </row>
     <row r="7" spans="2:23" ht="15">
-      <c r="B7" s="209" t="s">
+      <c r="B7" s="210" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="206"/>
@@ -15606,7 +15606,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="210" t="s">
+      <c r="F8" s="205" t="s">
         <v>41</v>
       </c>
       <c r="G8" s="206"/>
@@ -15618,7 +15618,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="210" t="s">
+      <c r="N8" s="205" t="s">
         <v>43</v>
       </c>
       <c r="O8" s="206"/>
@@ -15632,7 +15632,7 @@
       <c r="W8" s="1"/>
     </row>
     <row r="9" spans="2:23" ht="15">
-      <c r="B9" s="205" t="s">
+      <c r="B9" s="207" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="206"/>
@@ -15640,7 +15640,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="205" t="e">
+      <c r="F9" s="207" t="e">
         <f>CONCATENATE("Revenue ", Q39)</f>
         <v>#REF!</v>
       </c>
@@ -15654,7 +15654,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="205" t="e">
+      <c r="N9" s="207" t="e">
         <f>CONCATENATE("Revenue ", Q39)</f>
         <v>#REF!</v>
       </c>
@@ -15671,7 +15671,7 @@
       <c r="W9" s="1"/>
     </row>
     <row r="10" spans="2:23" ht="15">
-      <c r="B10" s="205" t="s">
+      <c r="B10" s="207" t="s">
         <v>151</v>
       </c>
       <c r="C10" s="206"/>
@@ -15679,7 +15679,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="205" t="e">
+      <c r="F10" s="207" t="e">
         <f>CONCATENATE("Revenue ", Z39)</f>
         <v>#REF!</v>
       </c>
@@ -15688,7 +15688,7 @@
         <v>0.03</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="205" t="e">
+      <c r="J10" s="207" t="e">
         <f>CONCATENATE("Revenue ", Z39)</f>
         <v>#REF!</v>
       </c>
@@ -15697,7 +15697,7 @@
         <v>0.05</v>
       </c>
       <c r="M10" s="1"/>
-      <c r="N10" s="205" t="e">
+      <c r="N10" s="207" t="e">
         <f>CONCATENATE("Revenue ", Z39)</f>
         <v>#REF!</v>
       </c>
@@ -15844,7 +15844,7 @@
         <v>0.09</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="205" t="e">
+      <c r="J14" s="207" t="e">
         <f>CONCATENATE("CapEx ", Z39)</f>
         <v>#REF!</v>
       </c>
@@ -15853,7 +15853,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="M14" s="1"/>
-      <c r="N14" s="205" t="e">
+      <c r="N14" s="207" t="e">
         <f>CONCATENATE("CapEx ", Z39)</f>
         <v>#REF!</v>
       </c>
@@ -15944,7 +15944,7 @@
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="15">
-      <c r="B17" s="210" t="s">
+      <c r="B17" s="205" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="206"/>
@@ -16055,7 +16055,7 @@
       <c r="A21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="209" t="s">
+      <c r="B21" s="210" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="206"/>
@@ -16350,7 +16350,7 @@
       <c r="W25" s="22"/>
     </row>
     <row r="26" spans="1:26" ht="15">
-      <c r="B26" s="208" t="s">
+      <c r="B26" s="212" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="206"/>
@@ -16693,7 +16693,7 @@
     </row>
     <row r="31" spans="1:26" ht="15">
       <c r="A31" s="1"/>
-      <c r="B31" s="205" t="s">
+      <c r="B31" s="207" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="206"/>
@@ -16750,7 +16750,7 @@
     </row>
     <row r="32" spans="1:26" ht="15">
       <c r="A32" s="1"/>
-      <c r="B32" s="205" t="s">
+      <c r="B32" s="207" t="s">
         <v>65</v>
       </c>
       <c r="C32" s="206"/>
@@ -16807,7 +16807,7 @@
     </row>
     <row r="33" spans="1:26" ht="15">
       <c r="A33" s="1"/>
-      <c r="B33" s="205" t="s">
+      <c r="B33" s="207" t="s">
         <v>43</v>
       </c>
       <c r="C33" s="206"/>
@@ -17075,7 +17075,7 @@
     </row>
     <row r="37" spans="1:26" ht="15">
       <c r="A37" s="1"/>
-      <c r="B37" s="205" t="s">
+      <c r="B37" s="207" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="206"/>
@@ -17132,7 +17132,7 @@
     </row>
     <row r="38" spans="1:26" ht="15">
       <c r="A38" s="1"/>
-      <c r="B38" s="205" t="s">
+      <c r="B38" s="207" t="s">
         <v>65</v>
       </c>
       <c r="C38" s="206"/>
@@ -17189,7 +17189,7 @@
     </row>
     <row r="39" spans="1:26" ht="15">
       <c r="A39" s="1"/>
-      <c r="B39" s="205" t="s">
+      <c r="B39" s="207" t="s">
         <v>43</v>
       </c>
       <c r="C39" s="206"/>
@@ -17271,6 +17271,17 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:D32"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="N14:O14"/>
     <mergeCell ref="B2:D2"/>
@@ -17285,17 +17296,6 @@
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:D32"/>
   </mergeCells>
   <conditionalFormatting sqref="K5:L5">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">

</xml_diff>